<commit_message>
Agregadas 2 tablas para general
</commit_message>
<xml_diff>
--- a/Data_Cobertura_Historica.xlsx
+++ b/Data_Cobertura_Historica.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3339" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="56">
   <si>
     <t>Distribuidora</t>
   </si>
@@ -188,6 +188,12 @@
   <si>
     <t>Fecha Generacion del …</t>
   </si>
+  <si>
+    <t>COBERTURA HISTORICA - GENERAL x Mesas</t>
+  </si>
+  <si>
+    <t>COB. HIST. - GEBERAL x Mes</t>
+  </si>
 </sst>
 </file>
 
@@ -280,6 +286,31 @@
     <tableColumn id="2" name="MES"/>
     <tableColumn id="3" name="Categoria"/>
     <tableColumn id="4" name="Clientes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="O3:R160" totalsRowShown="0">
+  <autoFilter ref="O3:R160"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Distribuidora"/>
+    <tableColumn id="2" name="MES"/>
+    <tableColumn id="3" name="Mesa"/>
+    <tableColumn id="4" name="Clientes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="U3:W77" totalsRowShown="0">
+  <autoFilter ref="U3:W77"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Distribuidora"/>
+    <tableColumn id="2" name="MES"/>
+    <tableColumn id="3" name="Clientes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -548,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L612"/>
+  <dimension ref="B1:W612"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,9 +591,11 @@
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>51</v>
       </c>
@@ -576,8 +609,19 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="U1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -605,8 +649,29 @@
       <c r="L3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" t="s">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -634,8 +699,29 @@
       <c r="L4">
         <v>312</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4">
+        <v>4</v>
+      </c>
+      <c r="U4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V4" t="s">
+        <v>6</v>
+      </c>
+      <c r="W4">
+        <v>3335</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -663,8 +749,29 @@
       <c r="L5">
         <v>289</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="U5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V5" t="s">
+        <v>12</v>
+      </c>
+      <c r="W5">
+        <v>3438</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -692,8 +799,29 @@
       <c r="L6">
         <v>363</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="U6" t="s">
+        <v>5</v>
+      </c>
+      <c r="V6" t="s">
+        <v>13</v>
+      </c>
+      <c r="W6">
+        <v>3632</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -721,8 +849,29 @@
       <c r="L7">
         <v>328</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="U7" t="s">
+        <v>5</v>
+      </c>
+      <c r="V7" t="s">
+        <v>14</v>
+      </c>
+      <c r="W7">
+        <v>3875</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -750,8 +899,29 @@
       <c r="L8">
         <v>410</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8">
+        <v>128</v>
+      </c>
+      <c r="U8" t="s">
+        <v>5</v>
+      </c>
+      <c r="V8" t="s">
+        <v>15</v>
+      </c>
+      <c r="W8">
+        <v>4006</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -779,8 +949,29 @@
       <c r="L9">
         <v>407</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9">
+        <v>37</v>
+      </c>
+      <c r="U9" t="s">
+        <v>5</v>
+      </c>
+      <c r="V9" t="s">
+        <v>16</v>
+      </c>
+      <c r="W9">
+        <v>3907</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -808,8 +999,29 @@
       <c r="L10">
         <v>374</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R10">
+        <v>71</v>
+      </c>
+      <c r="U10" t="s">
+        <v>5</v>
+      </c>
+      <c r="V10" t="s">
+        <v>17</v>
+      </c>
+      <c r="W10">
+        <v>3524</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -837,8 +1049,29 @@
       <c r="L11">
         <v>427</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>21</v>
+      </c>
+      <c r="R11">
+        <v>2371</v>
+      </c>
+      <c r="U11" t="s">
+        <v>5</v>
+      </c>
+      <c r="V11" t="s">
+        <v>18</v>
+      </c>
+      <c r="W11">
+        <v>3578</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>5</v>
       </c>
@@ -866,8 +1099,29 @@
       <c r="L12">
         <v>385</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>21</v>
+      </c>
+      <c r="R12">
+        <v>2175</v>
+      </c>
+      <c r="U12" t="s">
+        <v>5</v>
+      </c>
+      <c r="V12" t="s">
+        <v>19</v>
+      </c>
+      <c r="W12">
+        <v>3856</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -895,8 +1149,29 @@
       <c r="L13">
         <v>406</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>21</v>
+      </c>
+      <c r="R13">
+        <v>2077</v>
+      </c>
+      <c r="U13" t="s">
+        <v>5</v>
+      </c>
+      <c r="V13" t="s">
+        <v>23</v>
+      </c>
+      <c r="W13">
+        <v>3644</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -924,8 +1199,29 @@
       <c r="L14">
         <v>423</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>21</v>
+      </c>
+      <c r="R14">
+        <v>1883</v>
+      </c>
+      <c r="U14" t="s">
+        <v>5</v>
+      </c>
+      <c r="V14" t="s">
+        <v>24</v>
+      </c>
+      <c r="W14">
+        <v>3551</v>
+      </c>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>5</v>
       </c>
@@ -953,8 +1249,29 @@
       <c r="L15">
         <v>329</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>21</v>
+      </c>
+      <c r="R15">
+        <v>1226</v>
+      </c>
+      <c r="U15" t="s">
+        <v>5</v>
+      </c>
+      <c r="V15" t="s">
+        <v>25</v>
+      </c>
+      <c r="W15">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -982,8 +1299,29 @@
       <c r="L16">
         <v>300</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16">
+        <v>1742</v>
+      </c>
+      <c r="U16" t="s">
+        <v>5</v>
+      </c>
+      <c r="V16" t="s">
+        <v>26</v>
+      </c>
+      <c r="W16">
+        <v>2695</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>5</v>
       </c>
@@ -1011,8 +1349,29 @@
       <c r="L17">
         <v>289</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>5</v>
+      </c>
+      <c r="P17" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>21</v>
+      </c>
+      <c r="R17">
+        <v>1360</v>
+      </c>
+      <c r="U17" t="s">
+        <v>5</v>
+      </c>
+      <c r="V17" t="s">
+        <v>27</v>
+      </c>
+      <c r="W17">
+        <v>3077</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -1040,8 +1399,29 @@
       <c r="L18">
         <v>247</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P18" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>22</v>
+      </c>
+      <c r="R18">
+        <v>1506</v>
+      </c>
+      <c r="U18" t="s">
+        <v>5</v>
+      </c>
+      <c r="V18" t="s">
+        <v>28</v>
+      </c>
+      <c r="W18">
+        <v>2595</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -1069,8 +1449,29 @@
       <c r="L19">
         <v>2723</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>5</v>
+      </c>
+      <c r="P19" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>22</v>
+      </c>
+      <c r="R19">
+        <v>1471</v>
+      </c>
+      <c r="U19" t="s">
+        <v>5</v>
+      </c>
+      <c r="V19" t="s">
+        <v>29</v>
+      </c>
+      <c r="W19">
+        <v>2768</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -1098,8 +1499,29 @@
       <c r="L20">
         <v>2661</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>22</v>
+      </c>
+      <c r="R20">
+        <v>1471</v>
+      </c>
+      <c r="U20" t="s">
+        <v>31</v>
+      </c>
+      <c r="V20" t="s">
+        <v>6</v>
+      </c>
+      <c r="W20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -1127,8 +1549,29 @@
       <c r="L21">
         <v>2838</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>5</v>
+      </c>
+      <c r="P21" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21">
+        <v>1346</v>
+      </c>
+      <c r="U21" t="s">
+        <v>31</v>
+      </c>
+      <c r="V21" t="s">
+        <v>12</v>
+      </c>
+      <c r="W21">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>5</v>
       </c>
@@ -1156,8 +1599,29 @@
       <c r="L22">
         <v>3045</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O22" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>22</v>
+      </c>
+      <c r="R22">
+        <v>1440</v>
+      </c>
+      <c r="U22" t="s">
+        <v>31</v>
+      </c>
+      <c r="V22" t="s">
+        <v>13</v>
+      </c>
+      <c r="W22">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>5</v>
       </c>
@@ -1185,8 +1649,29 @@
       <c r="L23">
         <v>3051</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O23" t="s">
+        <v>5</v>
+      </c>
+      <c r="P23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>22</v>
+      </c>
+      <c r="R23">
+        <v>1314</v>
+      </c>
+      <c r="U23" t="s">
+        <v>31</v>
+      </c>
+      <c r="V23" t="s">
+        <v>14</v>
+      </c>
+      <c r="W23">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>5</v>
       </c>
@@ -1214,8 +1699,29 @@
       <c r="L24">
         <v>2984</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O24" t="s">
+        <v>5</v>
+      </c>
+      <c r="P24" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>22</v>
+      </c>
+      <c r="R24">
+        <v>1235</v>
+      </c>
+      <c r="U24" t="s">
+        <v>31</v>
+      </c>
+      <c r="V24" t="s">
+        <v>15</v>
+      </c>
+      <c r="W24">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>5</v>
       </c>
@@ -1243,8 +1749,29 @@
       <c r="L25">
         <v>2667</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O25" t="s">
+        <v>5</v>
+      </c>
+      <c r="P25" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>8</v>
+      </c>
+      <c r="R25">
+        <v>3335</v>
+      </c>
+      <c r="U25" t="s">
+        <v>31</v>
+      </c>
+      <c r="V25" t="s">
+        <v>16</v>
+      </c>
+      <c r="W25">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>5</v>
       </c>
@@ -1272,8 +1799,29 @@
       <c r="L26">
         <v>2817</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O26" t="s">
+        <v>5</v>
+      </c>
+      <c r="P26" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>8</v>
+      </c>
+      <c r="R26">
+        <v>3438</v>
+      </c>
+      <c r="U26" t="s">
+        <v>31</v>
+      </c>
+      <c r="V26" t="s">
+        <v>17</v>
+      </c>
+      <c r="W26">
+        <v>2294</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>5</v>
       </c>
@@ -1301,8 +1849,29 @@
       <c r="L27">
         <v>2847</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O27" t="s">
+        <v>5</v>
+      </c>
+      <c r="P27" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>8</v>
+      </c>
+      <c r="R27">
+        <v>3632</v>
+      </c>
+      <c r="U27" t="s">
+        <v>31</v>
+      </c>
+      <c r="V27" t="s">
+        <v>18</v>
+      </c>
+      <c r="W27">
+        <v>2157</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>5</v>
       </c>
@@ -1330,8 +1899,29 @@
       <c r="L28">
         <v>2831</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O28" t="s">
+        <v>5</v>
+      </c>
+      <c r="P28" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>8</v>
+      </c>
+      <c r="R28">
+        <v>3875</v>
+      </c>
+      <c r="U28" t="s">
+        <v>31</v>
+      </c>
+      <c r="V28" t="s">
+        <v>19</v>
+      </c>
+      <c r="W28">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>5</v>
       </c>
@@ -1359,8 +1949,29 @@
       <c r="L29">
         <v>2811</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O29" t="s">
+        <v>5</v>
+      </c>
+      <c r="P29" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>8</v>
+      </c>
+      <c r="R29">
+        <v>4006</v>
+      </c>
+      <c r="U29" t="s">
+        <v>31</v>
+      </c>
+      <c r="V29" t="s">
+        <v>23</v>
+      </c>
+      <c r="W29">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>5</v>
       </c>
@@ -1388,8 +1999,29 @@
       <c r="L30">
         <v>2653</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O30" t="s">
+        <v>5</v>
+      </c>
+      <c r="P30" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>8</v>
+      </c>
+      <c r="R30">
+        <v>3907</v>
+      </c>
+      <c r="U30" t="s">
+        <v>31</v>
+      </c>
+      <c r="V30" t="s">
+        <v>24</v>
+      </c>
+      <c r="W30">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>5</v>
       </c>
@@ -1417,8 +2049,29 @@
       <c r="L31">
         <v>2176</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O31" t="s">
+        <v>5</v>
+      </c>
+      <c r="P31" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>8</v>
+      </c>
+      <c r="R31">
+        <v>3524</v>
+      </c>
+      <c r="U31" t="s">
+        <v>31</v>
+      </c>
+      <c r="V31" t="s">
+        <v>25</v>
+      </c>
+      <c r="W31">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>5</v>
       </c>
@@ -1446,8 +2099,29 @@
       <c r="L32">
         <v>2297</v>
       </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O32" t="s">
+        <v>5</v>
+      </c>
+      <c r="P32" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>8</v>
+      </c>
+      <c r="R32">
+        <v>3578</v>
+      </c>
+      <c r="U32" t="s">
+        <v>31</v>
+      </c>
+      <c r="V32" t="s">
+        <v>26</v>
+      </c>
+      <c r="W32">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>5</v>
       </c>
@@ -1475,8 +2149,29 @@
       <c r="L33">
         <v>2000</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O33" t="s">
+        <v>5</v>
+      </c>
+      <c r="P33" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>30</v>
+      </c>
+      <c r="R33">
+        <v>2</v>
+      </c>
+      <c r="U33" t="s">
+        <v>31</v>
+      </c>
+      <c r="V33" t="s">
+        <v>27</v>
+      </c>
+      <c r="W33">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>5</v>
       </c>
@@ -1504,8 +2199,29 @@
       <c r="L34">
         <v>1372</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O34" t="s">
+        <v>5</v>
+      </c>
+      <c r="P34" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>21</v>
+      </c>
+      <c r="R34">
+        <v>1707</v>
+      </c>
+      <c r="U34" t="s">
+        <v>31</v>
+      </c>
+      <c r="V34" t="s">
+        <v>28</v>
+      </c>
+      <c r="W34">
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>5</v>
       </c>
@@ -1533,8 +2249,29 @@
       <c r="L35">
         <v>1335</v>
       </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O35" t="s">
+        <v>5</v>
+      </c>
+      <c r="P35" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>22</v>
+      </c>
+      <c r="R35">
+        <v>1059</v>
+      </c>
+      <c r="U35" t="s">
+        <v>31</v>
+      </c>
+      <c r="V35" t="s">
+        <v>29</v>
+      </c>
+      <c r="W35">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>5</v>
       </c>
@@ -1562,8 +2299,29 @@
       <c r="L36">
         <v>1349</v>
       </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O36" t="s">
+        <v>31</v>
+      </c>
+      <c r="P36" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>33</v>
+      </c>
+      <c r="R36">
+        <v>339</v>
+      </c>
+      <c r="U36" t="s">
+        <v>35</v>
+      </c>
+      <c r="V36" t="s">
+        <v>25</v>
+      </c>
+      <c r="W36">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>5</v>
       </c>
@@ -1591,8 +2349,29 @@
       <c r="L37">
         <v>1675</v>
       </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
+        <v>31</v>
+      </c>
+      <c r="P37" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>33</v>
+      </c>
+      <c r="R37">
+        <v>296</v>
+      </c>
+      <c r="U37" t="s">
+        <v>35</v>
+      </c>
+      <c r="V37" t="s">
+        <v>26</v>
+      </c>
+      <c r="W37">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>5</v>
       </c>
@@ -1620,8 +2399,29 @@
       <c r="L38">
         <v>1597</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O38" t="s">
+        <v>31</v>
+      </c>
+      <c r="P38" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>33</v>
+      </c>
+      <c r="R38">
+        <v>256</v>
+      </c>
+      <c r="U38" t="s">
+        <v>35</v>
+      </c>
+      <c r="V38" t="s">
+        <v>27</v>
+      </c>
+      <c r="W38">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>5</v>
       </c>
@@ -1649,8 +2449,29 @@
       <c r="L39">
         <v>1495</v>
       </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O39" t="s">
+        <v>31</v>
+      </c>
+      <c r="P39" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>33</v>
+      </c>
+      <c r="R39">
+        <v>250</v>
+      </c>
+      <c r="U39" t="s">
+        <v>35</v>
+      </c>
+      <c r="V39" t="s">
+        <v>28</v>
+      </c>
+      <c r="W39">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>5</v>
       </c>
@@ -1678,8 +2499,29 @@
       <c r="L40">
         <v>1439</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O40" t="s">
+        <v>31</v>
+      </c>
+      <c r="P40" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>33</v>
+      </c>
+      <c r="R40">
+        <v>235</v>
+      </c>
+      <c r="U40" t="s">
+        <v>35</v>
+      </c>
+      <c r="V40" t="s">
+        <v>29</v>
+      </c>
+      <c r="W40">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>5</v>
       </c>
@@ -1707,8 +2549,29 @@
       <c r="L41">
         <v>1447</v>
       </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O41" t="s">
+        <v>31</v>
+      </c>
+      <c r="P41" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>33</v>
+      </c>
+      <c r="R41">
+        <v>253</v>
+      </c>
+      <c r="U41" t="s">
+        <v>36</v>
+      </c>
+      <c r="V41" t="s">
+        <v>19</v>
+      </c>
+      <c r="W41">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>5</v>
       </c>
@@ -1736,8 +2599,29 @@
       <c r="L42">
         <v>1672</v>
       </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O42" t="s">
+        <v>31</v>
+      </c>
+      <c r="P42" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>33</v>
+      </c>
+      <c r="R42">
+        <v>213</v>
+      </c>
+      <c r="U42" t="s">
+        <v>36</v>
+      </c>
+      <c r="V42" t="s">
+        <v>23</v>
+      </c>
+      <c r="W42">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>5</v>
       </c>
@@ -1765,8 +2649,29 @@
       <c r="L43">
         <v>1419</v>
       </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O43" t="s">
+        <v>31</v>
+      </c>
+      <c r="P43" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>33</v>
+      </c>
+      <c r="R43">
+        <v>202</v>
+      </c>
+      <c r="U43" t="s">
+        <v>36</v>
+      </c>
+      <c r="V43" t="s">
+        <v>24</v>
+      </c>
+      <c r="W43">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>5</v>
       </c>
@@ -1794,8 +2699,29 @@
       <c r="L44">
         <v>1592</v>
       </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O44" t="s">
+        <v>31</v>
+      </c>
+      <c r="P44" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>33</v>
+      </c>
+      <c r="R44">
+        <v>256</v>
+      </c>
+      <c r="U44" t="s">
+        <v>36</v>
+      </c>
+      <c r="V44" t="s">
+        <v>25</v>
+      </c>
+      <c r="W44">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>5</v>
       </c>
@@ -1823,8 +2749,29 @@
       <c r="L45">
         <v>1069</v>
       </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O45" t="s">
+        <v>31</v>
+      </c>
+      <c r="P45" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>34</v>
+      </c>
+      <c r="R45">
+        <v>740</v>
+      </c>
+      <c r="U45" t="s">
+        <v>36</v>
+      </c>
+      <c r="V45" t="s">
+        <v>26</v>
+      </c>
+      <c r="W45">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>5</v>
       </c>
@@ -1852,8 +2799,29 @@
       <c r="L46">
         <v>1135</v>
       </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O46" t="s">
+        <v>31</v>
+      </c>
+      <c r="P46" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>34</v>
+      </c>
+      <c r="R46">
+        <v>745</v>
+      </c>
+      <c r="U46" t="s">
+        <v>36</v>
+      </c>
+      <c r="V46" t="s">
+        <v>27</v>
+      </c>
+      <c r="W46">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>5</v>
       </c>
@@ -1881,8 +2849,29 @@
       <c r="L47">
         <v>1486</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O47" t="s">
+        <v>31</v>
+      </c>
+      <c r="P47" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>34</v>
+      </c>
+      <c r="R47">
+        <v>729</v>
+      </c>
+      <c r="U47" t="s">
+        <v>36</v>
+      </c>
+      <c r="V47" t="s">
+        <v>28</v>
+      </c>
+      <c r="W47">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>5</v>
       </c>
@@ -1910,8 +2899,29 @@
       <c r="L48">
         <v>1108</v>
       </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O48" t="s">
+        <v>31</v>
+      </c>
+      <c r="P48" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>34</v>
+      </c>
+      <c r="R48">
+        <v>724</v>
+      </c>
+      <c r="U48" t="s">
+        <v>36</v>
+      </c>
+      <c r="V48" t="s">
+        <v>29</v>
+      </c>
+      <c r="W48">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>5</v>
       </c>
@@ -1939,8 +2949,29 @@
       <c r="L49">
         <v>1469</v>
       </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O49" t="s">
+        <v>31</v>
+      </c>
+      <c r="P49" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>34</v>
+      </c>
+      <c r="R49">
+        <v>756</v>
+      </c>
+      <c r="U49" t="s">
+        <v>41</v>
+      </c>
+      <c r="V49" t="s">
+        <v>14</v>
+      </c>
+      <c r="W49">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>5</v>
       </c>
@@ -1968,8 +2999,29 @@
       <c r="L50">
         <v>1414</v>
       </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O50" t="s">
+        <v>31</v>
+      </c>
+      <c r="P50" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>34</v>
+      </c>
+      <c r="R50">
+        <v>726</v>
+      </c>
+      <c r="U50" t="s">
+        <v>41</v>
+      </c>
+      <c r="V50" t="s">
+        <v>15</v>
+      </c>
+      <c r="W50">
+        <v>2888</v>
+      </c>
+    </row>
+    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>5</v>
       </c>
@@ -1997,8 +3049,29 @@
       <c r="L51">
         <v>1598</v>
       </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O51" t="s">
+        <v>31</v>
+      </c>
+      <c r="P51" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>34</v>
+      </c>
+      <c r="R51">
+        <v>735</v>
+      </c>
+      <c r="U51" t="s">
+        <v>41</v>
+      </c>
+      <c r="V51" t="s">
+        <v>16</v>
+      </c>
+      <c r="W51">
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>5</v>
       </c>
@@ -2026,8 +3099,29 @@
       <c r="L52">
         <v>1679</v>
       </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O52" t="s">
+        <v>31</v>
+      </c>
+      <c r="P52" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>34</v>
+      </c>
+      <c r="R52">
+        <v>632</v>
+      </c>
+      <c r="U52" t="s">
+        <v>41</v>
+      </c>
+      <c r="V52" t="s">
+        <v>17</v>
+      </c>
+      <c r="W52">
+        <v>5466</v>
+      </c>
+    </row>
+    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>5</v>
       </c>
@@ -2055,8 +3149,29 @@
       <c r="L53">
         <v>1926</v>
       </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O53" t="s">
+        <v>31</v>
+      </c>
+      <c r="P53" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>34</v>
+      </c>
+      <c r="R53">
+        <v>760</v>
+      </c>
+      <c r="U53" t="s">
+        <v>41</v>
+      </c>
+      <c r="V53" t="s">
+        <v>18</v>
+      </c>
+      <c r="W53">
+        <v>5768</v>
+      </c>
+    </row>
+    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>5</v>
       </c>
@@ -2084,8 +3199,29 @@
       <c r="L54">
         <v>1754</v>
       </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O54" t="s">
+        <v>31</v>
+      </c>
+      <c r="P54" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>32</v>
+      </c>
+      <c r="R54">
+        <v>1000</v>
+      </c>
+      <c r="U54" t="s">
+        <v>41</v>
+      </c>
+      <c r="V54" t="s">
+        <v>19</v>
+      </c>
+      <c r="W54">
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>5</v>
       </c>
@@ -2113,8 +3249,29 @@
       <c r="L55">
         <v>1553</v>
       </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O55" t="s">
+        <v>31</v>
+      </c>
+      <c r="P55" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>32</v>
+      </c>
+      <c r="R55">
+        <v>1055</v>
+      </c>
+      <c r="U55" t="s">
+        <v>41</v>
+      </c>
+      <c r="V55" t="s">
+        <v>23</v>
+      </c>
+      <c r="W55">
+        <v>6205</v>
+      </c>
+    </row>
+    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>5</v>
       </c>
@@ -2142,8 +3299,29 @@
       <c r="L56">
         <v>1629</v>
       </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O56" t="s">
+        <v>31</v>
+      </c>
+      <c r="P56" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>32</v>
+      </c>
+      <c r="R56">
+        <v>1147</v>
+      </c>
+      <c r="U56" t="s">
+        <v>41</v>
+      </c>
+      <c r="V56" t="s">
+        <v>24</v>
+      </c>
+      <c r="W56">
+        <v>6118</v>
+      </c>
+    </row>
+    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>5</v>
       </c>
@@ -2171,8 +3349,29 @@
       <c r="L57">
         <v>1695</v>
       </c>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O57" t="s">
+        <v>31</v>
+      </c>
+      <c r="P57" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>32</v>
+      </c>
+      <c r="R57">
+        <v>1135</v>
+      </c>
+      <c r="U57" t="s">
+        <v>41</v>
+      </c>
+      <c r="V57" t="s">
+        <v>25</v>
+      </c>
+      <c r="W57">
+        <v>5730</v>
+      </c>
+    </row>
+    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>5</v>
       </c>
@@ -2200,8 +3399,29 @@
       <c r="L58">
         <v>1563</v>
       </c>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O58" t="s">
+        <v>31</v>
+      </c>
+      <c r="P58" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>32</v>
+      </c>
+      <c r="R58">
+        <v>1186</v>
+      </c>
+      <c r="U58" t="s">
+        <v>41</v>
+      </c>
+      <c r="V58" t="s">
+        <v>26</v>
+      </c>
+      <c r="W58">
+        <v>6901</v>
+      </c>
+    </row>
+    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>5</v>
       </c>
@@ -2229,8 +3449,29 @@
       <c r="L59">
         <v>1508</v>
       </c>
-    </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O59" t="s">
+        <v>31</v>
+      </c>
+      <c r="P59" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>32</v>
+      </c>
+      <c r="R59">
+        <v>1244</v>
+      </c>
+      <c r="U59" t="s">
+        <v>41</v>
+      </c>
+      <c r="V59" t="s">
+        <v>27</v>
+      </c>
+      <c r="W59">
+        <v>6185</v>
+      </c>
+    </row>
+    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>5</v>
       </c>
@@ -2258,8 +3499,29 @@
       <c r="L60">
         <v>1347</v>
       </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O60" t="s">
+        <v>31</v>
+      </c>
+      <c r="P60" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>32</v>
+      </c>
+      <c r="R60">
+        <v>1288</v>
+      </c>
+      <c r="U60" t="s">
+        <v>41</v>
+      </c>
+      <c r="V60" t="s">
+        <v>28</v>
+      </c>
+      <c r="W60">
+        <v>7217</v>
+      </c>
+    </row>
+    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>5</v>
       </c>
@@ -2287,8 +3549,29 @@
       <c r="L61">
         <v>1155</v>
       </c>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O61" t="s">
+        <v>31</v>
+      </c>
+      <c r="P61" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>32</v>
+      </c>
+      <c r="R61">
+        <v>1179</v>
+      </c>
+      <c r="U61" t="s">
+        <v>41</v>
+      </c>
+      <c r="V61" t="s">
+        <v>29</v>
+      </c>
+      <c r="W61">
+        <v>5375</v>
+      </c>
+    </row>
+    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>5</v>
       </c>
@@ -2316,8 +3599,29 @@
       <c r="L62">
         <v>1340</v>
       </c>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O62" t="s">
+        <v>31</v>
+      </c>
+      <c r="P62" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>32</v>
+      </c>
+      <c r="R62">
+        <v>1192</v>
+      </c>
+      <c r="U62" t="s">
+        <v>46</v>
+      </c>
+      <c r="V62" t="s">
+        <v>6</v>
+      </c>
+      <c r="W62">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>5</v>
       </c>
@@ -2345,8 +3649,29 @@
       <c r="L63">
         <v>1125</v>
       </c>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P63" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>32</v>
+      </c>
+      <c r="R63">
+        <v>1159</v>
+      </c>
+      <c r="U63" t="s">
+        <v>46</v>
+      </c>
+      <c r="V63" t="s">
+        <v>12</v>
+      </c>
+      <c r="W63">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>5</v>
       </c>
@@ -2374,8 +3699,29 @@
       <c r="L64">
         <v>240</v>
       </c>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O64" t="s">
+        <v>31</v>
+      </c>
+      <c r="P64" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>32</v>
+      </c>
+      <c r="R64">
+        <v>1164</v>
+      </c>
+      <c r="U64" t="s">
+        <v>46</v>
+      </c>
+      <c r="V64" t="s">
+        <v>13</v>
+      </c>
+      <c r="W64">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="65" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>5</v>
       </c>
@@ -2403,8 +3749,29 @@
       <c r="L65">
         <v>2232</v>
       </c>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O65" t="s">
+        <v>31</v>
+      </c>
+      <c r="P65" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>32</v>
+      </c>
+      <c r="R65">
+        <v>1140</v>
+      </c>
+      <c r="U65" t="s">
+        <v>46</v>
+      </c>
+      <c r="V65" t="s">
+        <v>14</v>
+      </c>
+      <c r="W65">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="66" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>5</v>
       </c>
@@ -2432,8 +3799,29 @@
       <c r="L66">
         <v>913</v>
       </c>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O66" t="s">
+        <v>31</v>
+      </c>
+      <c r="P66" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>32</v>
+      </c>
+      <c r="R66">
+        <v>1176</v>
+      </c>
+      <c r="U66" t="s">
+        <v>46</v>
+      </c>
+      <c r="V66" t="s">
+        <v>15</v>
+      </c>
+      <c r="W66">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="67" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>5</v>
       </c>
@@ -2461,8 +3849,29 @@
       <c r="L67">
         <v>902</v>
       </c>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O67" t="s">
+        <v>31</v>
+      </c>
+      <c r="P67" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>32</v>
+      </c>
+      <c r="R67">
+        <v>1132</v>
+      </c>
+      <c r="U67" t="s">
+        <v>46</v>
+      </c>
+      <c r="V67" t="s">
+        <v>16</v>
+      </c>
+      <c r="W67">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="68" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>5</v>
       </c>
@@ -2490,8 +3899,29 @@
       <c r="L68">
         <v>79</v>
       </c>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O68" t="s">
+        <v>31</v>
+      </c>
+      <c r="P68" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>32</v>
+      </c>
+      <c r="R68">
+        <v>1310</v>
+      </c>
+      <c r="U68" t="s">
+        <v>46</v>
+      </c>
+      <c r="V68" t="s">
+        <v>17</v>
+      </c>
+      <c r="W68">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="69" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>5</v>
       </c>
@@ -2519,8 +3949,29 @@
       <c r="L69">
         <v>97</v>
       </c>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O69" t="s">
+        <v>31</v>
+      </c>
+      <c r="P69" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>30</v>
+      </c>
+      <c r="R69">
+        <v>201</v>
+      </c>
+      <c r="U69" t="s">
+        <v>46</v>
+      </c>
+      <c r="V69" t="s">
+        <v>18</v>
+      </c>
+      <c r="W69">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="70" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>5</v>
       </c>
@@ -2548,8 +3999,29 @@
       <c r="L70">
         <v>90</v>
       </c>
-    </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O70" t="s">
+        <v>31</v>
+      </c>
+      <c r="P70" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>34</v>
+      </c>
+      <c r="R70">
+        <v>370</v>
+      </c>
+      <c r="U70" t="s">
+        <v>46</v>
+      </c>
+      <c r="V70" t="s">
+        <v>19</v>
+      </c>
+      <c r="W70">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="71" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>5</v>
       </c>
@@ -2577,8 +4049,29 @@
       <c r="L71">
         <v>111</v>
       </c>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O71" t="s">
+        <v>31</v>
+      </c>
+      <c r="P71" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>32</v>
+      </c>
+      <c r="R71">
+        <v>1290</v>
+      </c>
+      <c r="U71" t="s">
+        <v>46</v>
+      </c>
+      <c r="V71" t="s">
+        <v>23</v>
+      </c>
+      <c r="W71">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="72" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>5</v>
       </c>
@@ -2606,8 +4099,29 @@
       <c r="L72">
         <v>141</v>
       </c>
-    </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O72" t="s">
+        <v>35</v>
+      </c>
+      <c r="P72" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>21</v>
+      </c>
+      <c r="R72">
+        <v>1048</v>
+      </c>
+      <c r="U72" t="s">
+        <v>46</v>
+      </c>
+      <c r="V72" t="s">
+        <v>24</v>
+      </c>
+      <c r="W72">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="73" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>5</v>
       </c>
@@ -2635,8 +4149,29 @@
       <c r="L73">
         <v>153</v>
       </c>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O73" t="s">
+        <v>35</v>
+      </c>
+      <c r="P73" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>21</v>
+      </c>
+      <c r="R73">
+        <v>1413</v>
+      </c>
+      <c r="U73" t="s">
+        <v>46</v>
+      </c>
+      <c r="V73" t="s">
+        <v>25</v>
+      </c>
+      <c r="W73">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="74" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>5</v>
       </c>
@@ -2664,8 +4199,29 @@
       <c r="L74">
         <v>232</v>
       </c>
-    </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O74" t="s">
+        <v>35</v>
+      </c>
+      <c r="P74" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>21</v>
+      </c>
+      <c r="R74">
+        <v>1240</v>
+      </c>
+      <c r="U74" t="s">
+        <v>46</v>
+      </c>
+      <c r="V74" t="s">
+        <v>26</v>
+      </c>
+      <c r="W74">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="75" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>5</v>
       </c>
@@ -2693,8 +4249,29 @@
       <c r="L75">
         <v>246</v>
       </c>
-    </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O75" t="s">
+        <v>35</v>
+      </c>
+      <c r="P75" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>21</v>
+      </c>
+      <c r="R75">
+        <v>1523</v>
+      </c>
+      <c r="U75" t="s">
+        <v>46</v>
+      </c>
+      <c r="V75" t="s">
+        <v>27</v>
+      </c>
+      <c r="W75">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="76" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>5</v>
       </c>
@@ -2722,8 +4299,29 @@
       <c r="L76">
         <v>218</v>
       </c>
-    </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O76" t="s">
+        <v>35</v>
+      </c>
+      <c r="P76" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>21</v>
+      </c>
+      <c r="R76">
+        <v>1345</v>
+      </c>
+      <c r="U76" t="s">
+        <v>46</v>
+      </c>
+      <c r="V76" t="s">
+        <v>28</v>
+      </c>
+      <c r="W76">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="77" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>5</v>
       </c>
@@ -2751,8 +4349,29 @@
       <c r="L77">
         <v>254</v>
       </c>
-    </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O77" t="s">
+        <v>36</v>
+      </c>
+      <c r="P77" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>40</v>
+      </c>
+      <c r="R77">
+        <v>1</v>
+      </c>
+      <c r="U77" t="s">
+        <v>46</v>
+      </c>
+      <c r="V77" t="s">
+        <v>29</v>
+      </c>
+      <c r="W77">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="78" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>5</v>
       </c>
@@ -2780,8 +4399,20 @@
       <c r="L78">
         <v>267</v>
       </c>
-    </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O78" t="s">
+        <v>36</v>
+      </c>
+      <c r="P78" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>38</v>
+      </c>
+      <c r="R78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>5</v>
       </c>
@@ -2809,8 +4440,20 @@
       <c r="L79">
         <v>221</v>
       </c>
-    </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O79" t="s">
+        <v>36</v>
+      </c>
+      <c r="P79" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>38</v>
+      </c>
+      <c r="R79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>5</v>
       </c>
@@ -2838,8 +4481,20 @@
       <c r="L80">
         <v>236</v>
       </c>
-    </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O80" t="s">
+        <v>36</v>
+      </c>
+      <c r="P80" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>38</v>
+      </c>
+      <c r="R80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>5</v>
       </c>
@@ -2867,8 +4522,20 @@
       <c r="L81">
         <v>232</v>
       </c>
-    </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O81" t="s">
+        <v>36</v>
+      </c>
+      <c r="P81" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>38</v>
+      </c>
+      <c r="R81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>5</v>
       </c>
@@ -2896,8 +4563,20 @@
       <c r="L82">
         <v>223</v>
       </c>
-    </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O82" t="s">
+        <v>36</v>
+      </c>
+      <c r="P82" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>39</v>
+      </c>
+      <c r="R82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>5</v>
       </c>
@@ -2925,8 +4604,20 @@
       <c r="L83">
         <v>825</v>
       </c>
-    </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O83" t="s">
+        <v>36</v>
+      </c>
+      <c r="P83" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>39</v>
+      </c>
+      <c r="R83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>5</v>
       </c>
@@ -2954,8 +4645,20 @@
       <c r="L84">
         <v>892</v>
       </c>
-    </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O84" t="s">
+        <v>36</v>
+      </c>
+      <c r="P84" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>39</v>
+      </c>
+      <c r="R84">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>5</v>
       </c>
@@ -2983,8 +4686,20 @@
       <c r="L85">
         <v>975</v>
       </c>
-    </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O85" t="s">
+        <v>36</v>
+      </c>
+      <c r="P85" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>39</v>
+      </c>
+      <c r="R85">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>5</v>
       </c>
@@ -3012,8 +4727,20 @@
       <c r="L86">
         <v>982</v>
       </c>
-    </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O86" t="s">
+        <v>36</v>
+      </c>
+      <c r="P86" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>39</v>
+      </c>
+      <c r="R86">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>5</v>
       </c>
@@ -3041,8 +4768,20 @@
       <c r="L87">
         <v>992</v>
       </c>
-    </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O87" t="s">
+        <v>36</v>
+      </c>
+      <c r="P87" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>37</v>
+      </c>
+      <c r="R87">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="88" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>5</v>
       </c>
@@ -3070,8 +4809,20 @@
       <c r="L88">
         <v>1034</v>
       </c>
-    </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O88" t="s">
+        <v>36</v>
+      </c>
+      <c r="P88" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>37</v>
+      </c>
+      <c r="R88">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>5</v>
       </c>
@@ -3099,8 +4850,20 @@
       <c r="L89">
         <v>2002</v>
       </c>
-    </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O89" t="s">
+        <v>36</v>
+      </c>
+      <c r="P89" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>37</v>
+      </c>
+      <c r="R89">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="90" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>5</v>
       </c>
@@ -3128,8 +4891,20 @@
       <c r="L90">
         <v>1895</v>
       </c>
-    </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O90" t="s">
+        <v>36</v>
+      </c>
+      <c r="P90" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>37</v>
+      </c>
+      <c r="R90">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="91" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>5</v>
       </c>
@@ -3157,8 +4932,20 @@
       <c r="L91">
         <v>1810</v>
       </c>
-    </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O91" t="s">
+        <v>36</v>
+      </c>
+      <c r="P91" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>37</v>
+      </c>
+      <c r="R91">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="92" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>5</v>
       </c>
@@ -3186,8 +4973,20 @@
       <c r="L92">
         <v>1804</v>
       </c>
-    </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O92" t="s">
+        <v>36</v>
+      </c>
+      <c r="P92" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>37</v>
+      </c>
+      <c r="R92">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="93" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>5</v>
       </c>
@@ -3215,8 +5014,20 @@
       <c r="L93">
         <v>1795</v>
       </c>
-    </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O93" t="s">
+        <v>36</v>
+      </c>
+      <c r="P93" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>37</v>
+      </c>
+      <c r="R93">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="94" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>5</v>
       </c>
@@ -3244,8 +5055,20 @@
       <c r="L94">
         <v>1769</v>
       </c>
-    </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O94" t="s">
+        <v>36</v>
+      </c>
+      <c r="P94" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>40</v>
+      </c>
+      <c r="R94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>5</v>
       </c>
@@ -3273,8 +5096,20 @@
       <c r="L95">
         <v>1806</v>
       </c>
-    </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O95" t="s">
+        <v>36</v>
+      </c>
+      <c r="P95" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>39</v>
+      </c>
+      <c r="R95">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="96" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>5</v>
       </c>
@@ -3302,8 +5137,20 @@
       <c r="L96">
         <v>1613</v>
       </c>
-    </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O96" t="s">
+        <v>36</v>
+      </c>
+      <c r="P96" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>37</v>
+      </c>
+      <c r="R96">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>5</v>
       </c>
@@ -3331,8 +5178,20 @@
       <c r="L97">
         <v>1900</v>
       </c>
-    </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O97" t="s">
+        <v>41</v>
+      </c>
+      <c r="P97" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>44</v>
+      </c>
+      <c r="R97">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>5</v>
       </c>
@@ -3360,8 +5219,20 @@
       <c r="L98">
         <v>312</v>
       </c>
-    </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O98" t="s">
+        <v>41</v>
+      </c>
+      <c r="P98" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>44</v>
+      </c>
+      <c r="R98">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="99" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>5</v>
       </c>
@@ -3389,8 +5260,20 @@
       <c r="L99">
         <v>323</v>
       </c>
-    </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O99" t="s">
+        <v>41</v>
+      </c>
+      <c r="P99" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>44</v>
+      </c>
+      <c r="R99">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="100" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>5</v>
       </c>
@@ -3418,8 +5301,20 @@
       <c r="L100">
         <v>326</v>
       </c>
-    </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O100" t="s">
+        <v>41</v>
+      </c>
+      <c r="P100" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>44</v>
+      </c>
+      <c r="R100">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="101" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>5</v>
       </c>
@@ -3447,8 +5342,20 @@
       <c r="L101">
         <v>435</v>
       </c>
-    </row>
-    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O101" t="s">
+        <v>41</v>
+      </c>
+      <c r="P101" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>44</v>
+      </c>
+      <c r="R101">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="102" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>5</v>
       </c>
@@ -3476,8 +5383,20 @@
       <c r="L102">
         <v>350</v>
       </c>
-    </row>
-    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O102" t="s">
+        <v>41</v>
+      </c>
+      <c r="P102" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>44</v>
+      </c>
+      <c r="R102">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="103" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>5</v>
       </c>
@@ -3505,8 +5424,20 @@
       <c r="L103">
         <v>385</v>
       </c>
-    </row>
-    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O103" t="s">
+        <v>41</v>
+      </c>
+      <c r="P103" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>44</v>
+      </c>
+      <c r="R103">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="104" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>5</v>
       </c>
@@ -3534,8 +5465,20 @@
       <c r="L104">
         <v>602</v>
       </c>
-    </row>
-    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O104" t="s">
+        <v>41</v>
+      </c>
+      <c r="P104" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>44</v>
+      </c>
+      <c r="R104">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="105" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>5</v>
       </c>
@@ -3563,8 +5506,20 @@
       <c r="L105">
         <v>516</v>
       </c>
-    </row>
-    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O105" t="s">
+        <v>41</v>
+      </c>
+      <c r="P105" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>44</v>
+      </c>
+      <c r="R105">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="106" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>5</v>
       </c>
@@ -3592,8 +5547,20 @@
       <c r="L106">
         <v>578</v>
       </c>
-    </row>
-    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O106" t="s">
+        <v>41</v>
+      </c>
+      <c r="P106" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>44</v>
+      </c>
+      <c r="R106">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="107" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>5</v>
       </c>
@@ -3621,8 +5588,20 @@
       <c r="L107">
         <v>552</v>
       </c>
-    </row>
-    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O107" t="s">
+        <v>41</v>
+      </c>
+      <c r="P107" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>45</v>
+      </c>
+      <c r="R107">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="108" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>5</v>
       </c>
@@ -3650,8 +5629,20 @@
       <c r="L108">
         <v>601</v>
       </c>
-    </row>
-    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O108" t="s">
+        <v>41</v>
+      </c>
+      <c r="P108" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>45</v>
+      </c>
+      <c r="R108">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="109" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>5</v>
       </c>
@@ -3679,8 +5670,20 @@
       <c r="L109">
         <v>509</v>
       </c>
-    </row>
-    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O109" t="s">
+        <v>41</v>
+      </c>
+      <c r="P109" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>45</v>
+      </c>
+      <c r="R109">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="110" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>5</v>
       </c>
@@ -3708,8 +5711,20 @@
       <c r="L110">
         <v>660</v>
       </c>
-    </row>
-    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O110" t="s">
+        <v>41</v>
+      </c>
+      <c r="P110" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>45</v>
+      </c>
+      <c r="R110">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="111" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>5</v>
       </c>
@@ -3737,8 +5752,20 @@
       <c r="L111">
         <v>607</v>
       </c>
-    </row>
-    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O111" t="s">
+        <v>41</v>
+      </c>
+      <c r="P111" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>45</v>
+      </c>
+      <c r="R111">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="112" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>5</v>
       </c>
@@ -3766,8 +5793,20 @@
       <c r="L112">
         <v>624</v>
       </c>
-    </row>
-    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O112" t="s">
+        <v>41</v>
+      </c>
+      <c r="P112" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>45</v>
+      </c>
+      <c r="R112">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="113" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>5</v>
       </c>
@@ -3795,8 +5834,20 @@
       <c r="L113">
         <v>462</v>
       </c>
-    </row>
-    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O113" t="s">
+        <v>41</v>
+      </c>
+      <c r="P113" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>45</v>
+      </c>
+      <c r="R113">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="114" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>5</v>
       </c>
@@ -3824,8 +5875,20 @@
       <c r="L114">
         <v>523</v>
       </c>
-    </row>
-    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O114" t="s">
+        <v>41</v>
+      </c>
+      <c r="P114" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>45</v>
+      </c>
+      <c r="R114">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="115" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>5</v>
       </c>
@@ -3853,8 +5916,20 @@
       <c r="L115">
         <v>518</v>
       </c>
-    </row>
-    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O115" t="s">
+        <v>41</v>
+      </c>
+      <c r="P115" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>45</v>
+      </c>
+      <c r="R115">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="116" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>5</v>
       </c>
@@ -3882,8 +5957,20 @@
       <c r="L116">
         <v>582</v>
       </c>
-    </row>
-    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O116" t="s">
+        <v>41</v>
+      </c>
+      <c r="P116" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>45</v>
+      </c>
+      <c r="R116">
+        <v>2829</v>
+      </c>
+    </row>
+    <row r="117" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>5</v>
       </c>
@@ -3911,8 +5998,20 @@
       <c r="L117">
         <v>648</v>
       </c>
-    </row>
-    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O117" t="s">
+        <v>41</v>
+      </c>
+      <c r="P117" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>42</v>
+      </c>
+      <c r="R117">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="118" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>5</v>
       </c>
@@ -3940,8 +6039,20 @@
       <c r="L118">
         <v>680</v>
       </c>
-    </row>
-    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O118" t="s">
+        <v>41</v>
+      </c>
+      <c r="P118" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>42</v>
+      </c>
+      <c r="R118">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="119" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>5</v>
       </c>
@@ -3969,8 +6080,20 @@
       <c r="L119">
         <v>1312</v>
       </c>
-    </row>
-    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O119" t="s">
+        <v>41</v>
+      </c>
+      <c r="P119" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>42</v>
+      </c>
+      <c r="R119">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="120" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>5</v>
       </c>
@@ -3998,8 +6121,20 @@
       <c r="L120">
         <v>1235</v>
       </c>
-    </row>
-    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O120" t="s">
+        <v>41</v>
+      </c>
+      <c r="P120" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>42</v>
+      </c>
+      <c r="R120">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="121" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>5</v>
       </c>
@@ -4027,8 +6162,20 @@
       <c r="L121">
         <v>1315</v>
       </c>
-    </row>
-    <row r="122" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O121" t="s">
+        <v>41</v>
+      </c>
+      <c r="P121" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>42</v>
+      </c>
+      <c r="R121">
+        <v>2365</v>
+      </c>
+    </row>
+    <row r="122" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>5</v>
       </c>
@@ -4056,8 +6203,20 @@
       <c r="L122">
         <v>1265</v>
       </c>
-    </row>
-    <row r="123" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O122" t="s">
+        <v>41</v>
+      </c>
+      <c r="P122" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>42</v>
+      </c>
+      <c r="R122">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="123" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>5</v>
       </c>
@@ -4085,8 +6244,20 @@
       <c r="L123">
         <v>1317</v>
       </c>
-    </row>
-    <row r="124" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O123" t="s">
+        <v>41</v>
+      </c>
+      <c r="P123" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>42</v>
+      </c>
+      <c r="R123">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="124" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>5</v>
       </c>
@@ -4114,8 +6285,20 @@
       <c r="L124">
         <v>1151</v>
       </c>
-    </row>
-    <row r="125" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O124" t="s">
+        <v>41</v>
+      </c>
+      <c r="P124" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>42</v>
+      </c>
+      <c r="R124">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="125" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>31</v>
       </c>
@@ -4143,8 +6326,20 @@
       <c r="L125">
         <v>1218</v>
       </c>
-    </row>
-    <row r="126" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O125" t="s">
+        <v>41</v>
+      </c>
+      <c r="P125" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>42</v>
+      </c>
+      <c r="R125">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="126" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>31</v>
       </c>
@@ -4172,8 +6367,20 @@
       <c r="L126">
         <v>1134</v>
       </c>
-    </row>
-    <row r="127" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O126" t="s">
+        <v>41</v>
+      </c>
+      <c r="P126" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>42</v>
+      </c>
+      <c r="R126">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="127" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>31</v>
       </c>
@@ -4201,8 +6408,20 @@
       <c r="L127">
         <v>1202</v>
       </c>
-    </row>
-    <row r="128" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O127" t="s">
+        <v>41</v>
+      </c>
+      <c r="P127" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>42</v>
+      </c>
+      <c r="R127">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="128" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>31</v>
       </c>
@@ -4230,8 +6449,20 @@
       <c r="L128">
         <v>187</v>
       </c>
-    </row>
-    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O128" t="s">
+        <v>41</v>
+      </c>
+      <c r="P128" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q128" t="s">
+        <v>42</v>
+      </c>
+      <c r="R128">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="129" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>31</v>
       </c>
@@ -4259,8 +6490,20 @@
       <c r="L129">
         <v>1505</v>
       </c>
-    </row>
-    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O129" t="s">
+        <v>41</v>
+      </c>
+      <c r="P129" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q129" t="s">
+        <v>43</v>
+      </c>
+      <c r="R129">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="130" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>31</v>
       </c>
@@ -4288,8 +6531,20 @@
       <c r="L130">
         <v>485</v>
       </c>
-    </row>
-    <row r="131" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O130" t="s">
+        <v>41</v>
+      </c>
+      <c r="P130" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q130" t="s">
+        <v>43</v>
+      </c>
+      <c r="R130">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="131" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>31</v>
       </c>
@@ -4317,8 +6572,20 @@
       <c r="L131">
         <v>981</v>
       </c>
-    </row>
-    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O131" t="s">
+        <v>41</v>
+      </c>
+      <c r="P131" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>43</v>
+      </c>
+      <c r="R131">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="132" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>31</v>
       </c>
@@ -4346,8 +6613,20 @@
       <c r="L132">
         <v>56</v>
       </c>
-    </row>
-    <row r="133" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O132" t="s">
+        <v>41</v>
+      </c>
+      <c r="P132" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>43</v>
+      </c>
+      <c r="R132">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="133" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>31</v>
       </c>
@@ -4375,8 +6654,20 @@
       <c r="L133">
         <v>97</v>
       </c>
-    </row>
-    <row r="134" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O133" t="s">
+        <v>41</v>
+      </c>
+      <c r="P133" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>43</v>
+      </c>
+      <c r="R133">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="134" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>31</v>
       </c>
@@ -4404,8 +6695,20 @@
       <c r="L134">
         <v>77</v>
       </c>
-    </row>
-    <row r="135" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O134" t="s">
+        <v>41</v>
+      </c>
+      <c r="P134" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q134" t="s">
+        <v>43</v>
+      </c>
+      <c r="R134">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="135" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>31</v>
       </c>
@@ -4433,8 +6736,20 @@
       <c r="L135">
         <v>117</v>
       </c>
-    </row>
-    <row r="136" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O135" t="s">
+        <v>41</v>
+      </c>
+      <c r="P135" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>43</v>
+      </c>
+      <c r="R135">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="136" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>31</v>
       </c>
@@ -4462,8 +6777,20 @@
       <c r="L136">
         <v>920</v>
       </c>
-    </row>
-    <row r="137" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O136" t="s">
+        <v>41</v>
+      </c>
+      <c r="P136" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q136" t="s">
+        <v>43</v>
+      </c>
+      <c r="R136">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="137" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>31</v>
       </c>
@@ -4491,8 +6818,20 @@
       <c r="L137">
         <v>1288</v>
       </c>
-    </row>
-    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O137" t="s">
+        <v>41</v>
+      </c>
+      <c r="P137" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>43</v>
+      </c>
+      <c r="R137">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="138" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>31</v>
       </c>
@@ -4520,8 +6859,20 @@
       <c r="L138">
         <v>1059</v>
       </c>
-    </row>
-    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O138" t="s">
+        <v>41</v>
+      </c>
+      <c r="P138" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>43</v>
+      </c>
+      <c r="R138">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="139" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>31</v>
       </c>
@@ -4549,8 +6900,20 @@
       <c r="L139">
         <v>1350</v>
       </c>
-    </row>
-    <row r="140" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O139" t="s">
+        <v>41</v>
+      </c>
+      <c r="P139" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>43</v>
+      </c>
+      <c r="R139">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="140" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>31</v>
       </c>
@@ -4578,8 +6941,20 @@
       <c r="L140">
         <v>84</v>
       </c>
-    </row>
-    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O140" t="s">
+        <v>41</v>
+      </c>
+      <c r="P140" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q140" t="s">
+        <v>43</v>
+      </c>
+      <c r="R140">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="141" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>31</v>
       </c>
@@ -4607,8 +6982,20 @@
       <c r="L141">
         <v>239</v>
       </c>
-    </row>
-    <row r="142" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O141" t="s">
+        <v>41</v>
+      </c>
+      <c r="P141" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q141" t="s">
+        <v>44</v>
+      </c>
+      <c r="R141">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="142" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>31</v>
       </c>
@@ -4636,8 +7023,20 @@
       <c r="L142">
         <v>251</v>
       </c>
-    </row>
-    <row r="143" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O142" t="s">
+        <v>41</v>
+      </c>
+      <c r="P142" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>45</v>
+      </c>
+      <c r="R142">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="143" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>31</v>
       </c>
@@ -4665,8 +7064,20 @@
       <c r="L143">
         <v>290</v>
       </c>
-    </row>
-    <row r="144" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O143" t="s">
+        <v>41</v>
+      </c>
+      <c r="P143" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q143" t="s">
+        <v>42</v>
+      </c>
+      <c r="R143">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="144" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>31</v>
       </c>
@@ -4694,8 +7105,20 @@
       <c r="L144">
         <v>457</v>
       </c>
-    </row>
-    <row r="145" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O144" t="s">
+        <v>41</v>
+      </c>
+      <c r="P144" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>43</v>
+      </c>
+      <c r="R144">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="145" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>31</v>
       </c>
@@ -4723,8 +7146,20 @@
       <c r="L145">
         <v>714</v>
       </c>
-    </row>
-    <row r="146" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O145" t="s">
+        <v>46</v>
+      </c>
+      <c r="P145" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>48</v>
+      </c>
+      <c r="R145">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="146" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>31</v>
       </c>
@@ -4752,8 +7187,20 @@
       <c r="L146">
         <v>662</v>
       </c>
-    </row>
-    <row r="147" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O146" t="s">
+        <v>46</v>
+      </c>
+      <c r="P146" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q146" t="s">
+        <v>48</v>
+      </c>
+      <c r="R146">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="147" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>31</v>
       </c>
@@ -4781,8 +7228,20 @@
       <c r="L147">
         <v>754</v>
       </c>
-    </row>
-    <row r="148" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O147" t="s">
+        <v>46</v>
+      </c>
+      <c r="P147" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q147" t="s">
+        <v>48</v>
+      </c>
+      <c r="R147">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="148" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>31</v>
       </c>
@@ -4810,8 +7269,20 @@
       <c r="L148">
         <v>109</v>
       </c>
-    </row>
-    <row r="149" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O148" t="s">
+        <v>46</v>
+      </c>
+      <c r="P148" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q148" t="s">
+        <v>48</v>
+      </c>
+      <c r="R148">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="149" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>31</v>
       </c>
@@ -4839,8 +7310,20 @@
       <c r="L149">
         <v>1175</v>
       </c>
-    </row>
-    <row r="150" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O149" t="s">
+        <v>46</v>
+      </c>
+      <c r="P149" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q149" t="s">
+        <v>48</v>
+      </c>
+      <c r="R149">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="150" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>31</v>
       </c>
@@ -4868,8 +7351,20 @@
       <c r="L150">
         <v>223</v>
       </c>
-    </row>
-    <row r="151" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O150" t="s">
+        <v>46</v>
+      </c>
+      <c r="P150" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q150" t="s">
+        <v>48</v>
+      </c>
+      <c r="R150">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="151" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>31</v>
       </c>
@@ -4897,8 +7392,20 @@
       <c r="L151">
         <v>510</v>
       </c>
-    </row>
-    <row r="152" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O151" t="s">
+        <v>46</v>
+      </c>
+      <c r="P151" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q151" t="s">
+        <v>48</v>
+      </c>
+      <c r="R151">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="152" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>31</v>
       </c>
@@ -4926,8 +7433,20 @@
       <c r="L152">
         <v>7</v>
       </c>
-    </row>
-    <row r="153" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O152" t="s">
+        <v>46</v>
+      </c>
+      <c r="P152" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q152" t="s">
+        <v>48</v>
+      </c>
+      <c r="R152">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="153" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>31</v>
       </c>
@@ -4955,8 +7474,20 @@
       <c r="L153">
         <v>65</v>
       </c>
-    </row>
-    <row r="154" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O153" t="s">
+        <v>46</v>
+      </c>
+      <c r="P153" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q153" t="s">
+        <v>48</v>
+      </c>
+      <c r="R153">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="154" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>31</v>
       </c>
@@ -4984,8 +7515,20 @@
       <c r="L154">
         <v>66</v>
       </c>
-    </row>
-    <row r="155" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O154" t="s">
+        <v>46</v>
+      </c>
+      <c r="P154" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q154" t="s">
+        <v>48</v>
+      </c>
+      <c r="R154">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="155" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>31</v>
       </c>
@@ -5013,8 +7556,20 @@
       <c r="L155">
         <v>103</v>
       </c>
-    </row>
-    <row r="156" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O155" t="s">
+        <v>46</v>
+      </c>
+      <c r="P155" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q155" t="s">
+        <v>48</v>
+      </c>
+      <c r="R155">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="156" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>31</v>
       </c>
@@ -5042,8 +7597,20 @@
       <c r="L156">
         <v>158</v>
       </c>
-    </row>
-    <row r="157" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O156" t="s">
+        <v>46</v>
+      </c>
+      <c r="P156" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q156" t="s">
+        <v>48</v>
+      </c>
+      <c r="R156">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="157" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>31</v>
       </c>
@@ -5071,8 +7638,20 @@
       <c r="L157">
         <v>164</v>
       </c>
-    </row>
-    <row r="158" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O157" t="s">
+        <v>46</v>
+      </c>
+      <c r="P157" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q157" t="s">
+        <v>48</v>
+      </c>
+      <c r="R157">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="158" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>31</v>
       </c>
@@ -5100,8 +7679,20 @@
       <c r="L158">
         <v>173</v>
       </c>
-    </row>
-    <row r="159" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O158" t="s">
+        <v>46</v>
+      </c>
+      <c r="P158" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q158" t="s">
+        <v>48</v>
+      </c>
+      <c r="R158">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="159" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>31</v>
       </c>
@@ -5129,8 +7720,20 @@
       <c r="L159">
         <v>161</v>
       </c>
-    </row>
-    <row r="160" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O159" t="s">
+        <v>46</v>
+      </c>
+      <c r="P159" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q159" t="s">
+        <v>48</v>
+      </c>
+      <c r="R159">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="160" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>31</v>
       </c>
@@ -5157,6 +7760,18 @@
       </c>
       <c r="L160">
         <v>429</v>
+      </c>
+      <c r="O160" t="s">
+        <v>46</v>
+      </c>
+      <c r="P160" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q160" t="s">
+        <v>48</v>
+      </c>
+      <c r="R160">
+        <v>937</v>
       </c>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.25">
@@ -14512,15 +17127,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="I1:L1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="U1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Se corrigieron problemas de espacios
</commit_message>
<xml_diff>
--- a/Data_Cobertura_Historica.xlsx
+++ b/Data_Cobertura_Historica.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="53">
   <si>
     <t>Distribuidora</t>
   </si>
@@ -168,16 +168,7 @@
     <t>ZV</t>
   </si>
   <si>
-    <t xml:space="preserve">ADULT    </t>
-  </si>
-  <si>
     <t>(KCC ) Mesa 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAMILY   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">INFANT   </t>
   </si>
   <si>
     <t>COBERTURA HISTORICA x Mesa</t>
@@ -581,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W612"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,26 +588,26 @@
   <sheetData>
     <row r="1" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="O1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="U1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
@@ -5902,7 +5893,7 @@
         <v>21</v>
       </c>
       <c r="F115">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I115" t="s">
         <v>31</v>
@@ -5943,7 +5934,7 @@
         <v>22</v>
       </c>
       <c r="F116">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I116" t="s">
         <v>31</v>
@@ -6025,7 +6016,7 @@
         <v>21</v>
       </c>
       <c r="F118">
-        <v>1364</v>
+        <v>1345</v>
       </c>
       <c r="I118" t="s">
         <v>31</v>
@@ -6066,7 +6057,7 @@
         <v>22</v>
       </c>
       <c r="F119">
-        <v>903</v>
+        <v>886</v>
       </c>
       <c r="I119" t="s">
         <v>31</v>
@@ -6107,7 +6098,7 @@
         <v>21</v>
       </c>
       <c r="F120">
-        <v>627</v>
+        <v>618</v>
       </c>
       <c r="I120" t="s">
         <v>31</v>
@@ -6148,7 +6139,7 @@
         <v>22</v>
       </c>
       <c r="F121">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="I121" t="s">
         <v>31</v>
@@ -6230,7 +6221,7 @@
         <v>21</v>
       </c>
       <c r="F123">
-        <v>587</v>
+        <v>578</v>
       </c>
       <c r="I123" t="s">
         <v>31</v>
@@ -6271,7 +6262,7 @@
         <v>22</v>
       </c>
       <c r="F124">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="I124" t="s">
         <v>31</v>
@@ -7153,7 +7144,7 @@
         <v>6</v>
       </c>
       <c r="Q145" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R145">
         <v>1977</v>
@@ -7194,7 +7185,7 @@
         <v>12</v>
       </c>
       <c r="Q146" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R146">
         <v>1705</v>
@@ -7235,7 +7226,7 @@
         <v>13</v>
       </c>
       <c r="Q147" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R147">
         <v>1542</v>
@@ -7276,7 +7267,7 @@
         <v>14</v>
       </c>
       <c r="Q148" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R148">
         <v>1732</v>
@@ -7317,7 +7308,7 @@
         <v>15</v>
       </c>
       <c r="Q149" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R149">
         <v>1783</v>
@@ -7358,7 +7349,7 @@
         <v>16</v>
       </c>
       <c r="Q150" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R150">
         <v>1915</v>
@@ -7399,7 +7390,7 @@
         <v>17</v>
       </c>
       <c r="Q151" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R151">
         <v>1858</v>
@@ -7440,7 +7431,7 @@
         <v>18</v>
       </c>
       <c r="Q152" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R152">
         <v>1911</v>
@@ -7481,7 +7472,7 @@
         <v>19</v>
       </c>
       <c r="Q153" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R153">
         <v>1901</v>
@@ -7522,7 +7513,7 @@
         <v>23</v>
       </c>
       <c r="Q154" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R154">
         <v>1844</v>
@@ -7563,7 +7554,7 @@
         <v>24</v>
       </c>
       <c r="Q155" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R155">
         <v>1831</v>
@@ -7604,7 +7595,7 @@
         <v>25</v>
       </c>
       <c r="Q156" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R156">
         <v>1662</v>
@@ -7645,7 +7636,7 @@
         <v>26</v>
       </c>
       <c r="Q157" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R157">
         <v>1726</v>
@@ -7686,7 +7677,7 @@
         <v>27</v>
       </c>
       <c r="Q158" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R158">
         <v>1307</v>
@@ -7727,7 +7718,7 @@
         <v>28</v>
       </c>
       <c r="Q159" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R159">
         <v>1100</v>
@@ -7768,7 +7759,7 @@
         <v>29</v>
       </c>
       <c r="Q160" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R160">
         <v>937</v>
@@ -9972,7 +9963,7 @@
         <v>6</v>
       </c>
       <c r="K236" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L236">
         <v>265</v>
@@ -10001,7 +9992,7 @@
         <v>12</v>
       </c>
       <c r="K237" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L237">
         <v>244</v>
@@ -10030,7 +10021,7 @@
         <v>13</v>
       </c>
       <c r="K238" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L238">
         <v>245</v>
@@ -10059,7 +10050,7 @@
         <v>14</v>
       </c>
       <c r="K239" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L239">
         <v>284</v>
@@ -10088,7 +10079,7 @@
         <v>15</v>
       </c>
       <c r="K240" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L240">
         <v>286</v>
@@ -10117,7 +10108,7 @@
         <v>16</v>
       </c>
       <c r="K241" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L241">
         <v>274</v>
@@ -10146,7 +10137,7 @@
         <v>17</v>
       </c>
       <c r="K242" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L242">
         <v>295</v>
@@ -10175,7 +10166,7 @@
         <v>18</v>
       </c>
       <c r="K243" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L243">
         <v>297</v>
@@ -10204,7 +10195,7 @@
         <v>19</v>
       </c>
       <c r="K244" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L244">
         <v>337</v>
@@ -10233,7 +10224,7 @@
         <v>23</v>
       </c>
       <c r="K245" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L245">
         <v>310</v>
@@ -10262,7 +10253,7 @@
         <v>24</v>
       </c>
       <c r="K246" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L246">
         <v>374</v>
@@ -10291,7 +10282,7 @@
         <v>25</v>
       </c>
       <c r="K247" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L247">
         <v>275</v>
@@ -10320,7 +10311,7 @@
         <v>26</v>
       </c>
       <c r="K248" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L248">
         <v>279</v>
@@ -10349,7 +10340,7 @@
         <v>27</v>
       </c>
       <c r="K249" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L249">
         <v>196</v>
@@ -10378,7 +10369,7 @@
         <v>28</v>
       </c>
       <c r="K250" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L250">
         <v>176</v>
@@ -10407,7 +10398,7 @@
         <v>6</v>
       </c>
       <c r="K251" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L251">
         <v>1463</v>
@@ -10436,7 +10427,7 @@
         <v>12</v>
       </c>
       <c r="K252" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L252">
         <v>1253</v>
@@ -10465,7 +10456,7 @@
         <v>13</v>
       </c>
       <c r="K253" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L253">
         <v>1159</v>
@@ -10494,7 +10485,7 @@
         <v>14</v>
       </c>
       <c r="K254" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L254">
         <v>1322</v>
@@ -10523,7 +10514,7 @@
         <v>15</v>
       </c>
       <c r="K255" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L255">
         <v>1316</v>
@@ -10552,7 +10543,7 @@
         <v>16</v>
       </c>
       <c r="K256" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L256">
         <v>1515</v>
@@ -10581,7 +10572,7 @@
         <v>17</v>
       </c>
       <c r="K257" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L257">
         <v>1441</v>
@@ -10610,7 +10601,7 @@
         <v>18</v>
       </c>
       <c r="K258" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L258">
         <v>1449</v>
@@ -10630,7 +10621,7 @@
         <v>30</v>
       </c>
       <c r="F259">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="I259" t="s">
         <v>46</v>
@@ -10639,7 +10630,7 @@
         <v>19</v>
       </c>
       <c r="K259" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L259">
         <v>1427</v>
@@ -10668,7 +10659,7 @@
         <v>23</v>
       </c>
       <c r="K260" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L260">
         <v>1456</v>
@@ -10688,7 +10679,7 @@
         <v>32</v>
       </c>
       <c r="F261">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="I261" t="s">
         <v>46</v>
@@ -10697,7 +10688,7 @@
         <v>24</v>
       </c>
       <c r="K261" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L261">
         <v>1455</v>
@@ -10726,7 +10717,7 @@
         <v>25</v>
       </c>
       <c r="K262" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L262">
         <v>1303</v>
@@ -10755,7 +10746,7 @@
         <v>26</v>
       </c>
       <c r="K263" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L263">
         <v>1362</v>
@@ -10784,7 +10775,7 @@
         <v>27</v>
       </c>
       <c r="K264" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L264">
         <v>859</v>
@@ -10804,7 +10795,7 @@
         <v>30</v>
       </c>
       <c r="F265">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I265" t="s">
         <v>46</v>
@@ -10813,7 +10804,7 @@
         <v>28</v>
       </c>
       <c r="K265" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L265">
         <v>741</v>
@@ -10862,7 +10853,7 @@
         <v>32</v>
       </c>
       <c r="F267">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="I267" t="s">
         <v>46</v>
@@ -11277,7 +11268,7 @@
         <v>6</v>
       </c>
       <c r="K281" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L281">
         <v>1066</v>
@@ -11306,7 +11297,7 @@
         <v>12</v>
       </c>
       <c r="K282" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L282">
         <v>813</v>
@@ -11335,7 +11326,7 @@
         <v>13</v>
       </c>
       <c r="K283" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L283">
         <v>744</v>
@@ -11364,7 +11355,7 @@
         <v>14</v>
       </c>
       <c r="K284" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L284">
         <v>875</v>
@@ -11393,7 +11384,7 @@
         <v>15</v>
       </c>
       <c r="K285" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L285">
         <v>942</v>
@@ -11422,7 +11413,7 @@
         <v>16</v>
       </c>
       <c r="K286" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L286">
         <v>1031</v>
@@ -11451,7 +11442,7 @@
         <v>17</v>
       </c>
       <c r="K287" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L287">
         <v>953</v>
@@ -11480,7 +11471,7 @@
         <v>18</v>
       </c>
       <c r="K288" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L288">
         <v>974</v>
@@ -11509,7 +11500,7 @@
         <v>19</v>
       </c>
       <c r="K289" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L289">
         <v>1102</v>
@@ -11538,7 +11529,7 @@
         <v>23</v>
       </c>
       <c r="K290" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L290">
         <v>945</v>
@@ -11567,7 +11558,7 @@
         <v>24</v>
       </c>
       <c r="K291" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L291">
         <v>899</v>
@@ -11596,7 +11587,7 @@
         <v>25</v>
       </c>
       <c r="K292" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L292">
         <v>787</v>
@@ -11625,7 +11616,7 @@
         <v>26</v>
       </c>
       <c r="K293" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L293">
         <v>786</v>
@@ -11654,7 +11645,7 @@
         <v>27</v>
       </c>
       <c r="K294" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L294">
         <v>634</v>
@@ -11683,7 +11674,7 @@
         <v>28</v>
       </c>
       <c r="K295" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L295">
         <v>581</v>
@@ -11712,7 +11703,7 @@
         <v>29</v>
       </c>
       <c r="K296" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="L296">
         <v>127</v>
@@ -11741,7 +11732,7 @@
         <v>29</v>
       </c>
       <c r="K297" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="L297">
         <v>630</v>
@@ -11799,7 +11790,7 @@
         <v>29</v>
       </c>
       <c r="K299" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L299">
         <v>389</v>
@@ -16046,10 +16037,10 @@
         <v>6</v>
       </c>
       <c r="D549" t="s">
+        <v>7</v>
+      </c>
+      <c r="E549" t="s">
         <v>47</v>
-      </c>
-      <c r="E549" t="s">
-        <v>48</v>
       </c>
       <c r="F549">
         <v>265</v>
@@ -16063,10 +16054,10 @@
         <v>6</v>
       </c>
       <c r="D550" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E550" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F550">
         <v>1463</v>
@@ -16083,7 +16074,7 @@
         <v>10</v>
       </c>
       <c r="E551" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F551">
         <v>608</v>
@@ -16097,10 +16088,10 @@
         <v>6</v>
       </c>
       <c r="D552" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E552" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F552">
         <v>1066</v>
@@ -16114,10 +16105,10 @@
         <v>12</v>
       </c>
       <c r="D553" t="s">
+        <v>7</v>
+      </c>
+      <c r="E553" t="s">
         <v>47</v>
-      </c>
-      <c r="E553" t="s">
-        <v>48</v>
       </c>
       <c r="F553">
         <v>244</v>
@@ -16131,10 +16122,10 @@
         <v>12</v>
       </c>
       <c r="D554" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E554" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F554">
         <v>1253</v>
@@ -16151,7 +16142,7 @@
         <v>10</v>
       </c>
       <c r="E555" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F555">
         <v>530</v>
@@ -16165,10 +16156,10 @@
         <v>12</v>
       </c>
       <c r="D556" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E556" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F556">
         <v>813</v>
@@ -16182,10 +16173,10 @@
         <v>13</v>
       </c>
       <c r="D557" t="s">
+        <v>7</v>
+      </c>
+      <c r="E557" t="s">
         <v>47</v>
-      </c>
-      <c r="E557" t="s">
-        <v>48</v>
       </c>
       <c r="F557">
         <v>245</v>
@@ -16199,10 +16190,10 @@
         <v>13</v>
       </c>
       <c r="D558" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E558" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F558">
         <v>1159</v>
@@ -16219,7 +16210,7 @@
         <v>10</v>
       </c>
       <c r="E559" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F559">
         <v>514</v>
@@ -16233,10 +16224,10 @@
         <v>13</v>
       </c>
       <c r="D560" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E560" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F560">
         <v>744</v>
@@ -16250,10 +16241,10 @@
         <v>14</v>
       </c>
       <c r="D561" t="s">
+        <v>7</v>
+      </c>
+      <c r="E561" t="s">
         <v>47</v>
-      </c>
-      <c r="E561" t="s">
-        <v>48</v>
       </c>
       <c r="F561">
         <v>284</v>
@@ -16267,10 +16258,10 @@
         <v>14</v>
       </c>
       <c r="D562" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E562" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F562">
         <v>1322</v>
@@ -16287,7 +16278,7 @@
         <v>10</v>
       </c>
       <c r="E563" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F563">
         <v>708</v>
@@ -16301,10 +16292,10 @@
         <v>14</v>
       </c>
       <c r="D564" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E564" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F564">
         <v>875</v>
@@ -16318,10 +16309,10 @@
         <v>15</v>
       </c>
       <c r="D565" t="s">
+        <v>7</v>
+      </c>
+      <c r="E565" t="s">
         <v>47</v>
-      </c>
-      <c r="E565" t="s">
-        <v>48</v>
       </c>
       <c r="F565">
         <v>286</v>
@@ -16335,10 +16326,10 @@
         <v>15</v>
       </c>
       <c r="D566" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E566" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F566">
         <v>1316</v>
@@ -16355,7 +16346,7 @@
         <v>10</v>
       </c>
       <c r="E567" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F567">
         <v>684</v>
@@ -16369,10 +16360,10 @@
         <v>15</v>
       </c>
       <c r="D568" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E568" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F568">
         <v>942</v>
@@ -16386,10 +16377,10 @@
         <v>16</v>
       </c>
       <c r="D569" t="s">
+        <v>7</v>
+      </c>
+      <c r="E569" t="s">
         <v>47</v>
-      </c>
-      <c r="E569" t="s">
-        <v>48</v>
       </c>
       <c r="F569">
         <v>274</v>
@@ -16403,10 +16394,10 @@
         <v>16</v>
       </c>
       <c r="D570" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E570" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F570">
         <v>1515</v>
@@ -16423,7 +16414,7 @@
         <v>10</v>
       </c>
       <c r="E571" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F571">
         <v>599</v>
@@ -16437,10 +16428,10 @@
         <v>16</v>
       </c>
       <c r="D572" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E572" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F572">
         <v>1031</v>
@@ -16454,10 +16445,10 @@
         <v>17</v>
       </c>
       <c r="D573" t="s">
+        <v>7</v>
+      </c>
+      <c r="E573" t="s">
         <v>47</v>
-      </c>
-      <c r="E573" t="s">
-        <v>48</v>
       </c>
       <c r="F573">
         <v>295</v>
@@ -16471,10 +16462,10 @@
         <v>17</v>
       </c>
       <c r="D574" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E574" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F574">
         <v>1441</v>
@@ -16491,7 +16482,7 @@
         <v>10</v>
       </c>
       <c r="E575" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F575">
         <v>627</v>
@@ -16505,10 +16496,10 @@
         <v>17</v>
       </c>
       <c r="D576" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E576" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F576">
         <v>953</v>
@@ -16522,10 +16513,10 @@
         <v>18</v>
       </c>
       <c r="D577" t="s">
+        <v>7</v>
+      </c>
+      <c r="E577" t="s">
         <v>47</v>
-      </c>
-      <c r="E577" t="s">
-        <v>48</v>
       </c>
       <c r="F577">
         <v>297</v>
@@ -16539,10 +16530,10 @@
         <v>18</v>
       </c>
       <c r="D578" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E578" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F578">
         <v>1449</v>
@@ -16559,7 +16550,7 @@
         <v>10</v>
       </c>
       <c r="E579" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F579">
         <v>660</v>
@@ -16573,10 +16564,10 @@
         <v>18</v>
       </c>
       <c r="D580" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E580" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F580">
         <v>974</v>
@@ -16590,10 +16581,10 @@
         <v>19</v>
       </c>
       <c r="D581" t="s">
+        <v>7</v>
+      </c>
+      <c r="E581" t="s">
         <v>47</v>
-      </c>
-      <c r="E581" t="s">
-        <v>48</v>
       </c>
       <c r="F581">
         <v>337</v>
@@ -16607,10 +16598,10 @@
         <v>19</v>
       </c>
       <c r="D582" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E582" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F582">
         <v>1427</v>
@@ -16627,7 +16618,7 @@
         <v>10</v>
       </c>
       <c r="E583" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F583">
         <v>692</v>
@@ -16641,10 +16632,10 @@
         <v>19</v>
       </c>
       <c r="D584" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E584" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F584">
         <v>1102</v>
@@ -16658,10 +16649,10 @@
         <v>23</v>
       </c>
       <c r="D585" t="s">
+        <v>7</v>
+      </c>
+      <c r="E585" t="s">
         <v>47</v>
-      </c>
-      <c r="E585" t="s">
-        <v>48</v>
       </c>
       <c r="F585">
         <v>310</v>
@@ -16675,10 +16666,10 @@
         <v>23</v>
       </c>
       <c r="D586" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E586" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F586">
         <v>1456</v>
@@ -16695,7 +16686,7 @@
         <v>10</v>
       </c>
       <c r="E587" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F587">
         <v>667</v>
@@ -16709,10 +16700,10 @@
         <v>23</v>
       </c>
       <c r="D588" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E588" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F588">
         <v>945</v>
@@ -16726,10 +16717,10 @@
         <v>24</v>
       </c>
       <c r="D589" t="s">
+        <v>7</v>
+      </c>
+      <c r="E589" t="s">
         <v>47</v>
-      </c>
-      <c r="E589" t="s">
-        <v>48</v>
       </c>
       <c r="F589">
         <v>374</v>
@@ -16743,10 +16734,10 @@
         <v>24</v>
       </c>
       <c r="D590" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E590" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F590">
         <v>1455</v>
@@ -16763,7 +16754,7 @@
         <v>10</v>
       </c>
       <c r="E591" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F591">
         <v>659</v>
@@ -16777,10 +16768,10 @@
         <v>24</v>
       </c>
       <c r="D592" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E592" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F592">
         <v>899</v>
@@ -16794,10 +16785,10 @@
         <v>25</v>
       </c>
       <c r="D593" t="s">
+        <v>7</v>
+      </c>
+      <c r="E593" t="s">
         <v>47</v>
-      </c>
-      <c r="E593" t="s">
-        <v>48</v>
       </c>
       <c r="F593">
         <v>275</v>
@@ -16811,10 +16802,10 @@
         <v>25</v>
       </c>
       <c r="D594" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E594" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F594">
         <v>1303</v>
@@ -16831,7 +16822,7 @@
         <v>10</v>
       </c>
       <c r="E595" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F595">
         <v>364</v>
@@ -16845,10 +16836,10 @@
         <v>25</v>
       </c>
       <c r="D596" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E596" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F596">
         <v>787</v>
@@ -16862,10 +16853,10 @@
         <v>26</v>
       </c>
       <c r="D597" t="s">
+        <v>7</v>
+      </c>
+      <c r="E597" t="s">
         <v>47</v>
-      </c>
-      <c r="E597" t="s">
-        <v>48</v>
       </c>
       <c r="F597">
         <v>279</v>
@@ -16879,10 +16870,10 @@
         <v>26</v>
       </c>
       <c r="D598" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E598" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F598">
         <v>1362</v>
@@ -16899,7 +16890,7 @@
         <v>10</v>
       </c>
       <c r="E599" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F599">
         <v>572</v>
@@ -16913,10 +16904,10 @@
         <v>26</v>
       </c>
       <c r="D600" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E600" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F600">
         <v>786</v>
@@ -16930,10 +16921,10 @@
         <v>27</v>
       </c>
       <c r="D601" t="s">
+        <v>7</v>
+      </c>
+      <c r="E601" t="s">
         <v>47</v>
-      </c>
-      <c r="E601" t="s">
-        <v>48</v>
       </c>
       <c r="F601">
         <v>196</v>
@@ -16947,10 +16938,10 @@
         <v>27</v>
       </c>
       <c r="D602" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E602" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F602">
         <v>859</v>
@@ -16967,7 +16958,7 @@
         <v>10</v>
       </c>
       <c r="E603" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F603">
         <v>429</v>
@@ -16981,10 +16972,10 @@
         <v>27</v>
       </c>
       <c r="D604" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E604" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F604">
         <v>634</v>
@@ -16998,10 +16989,10 @@
         <v>28</v>
       </c>
       <c r="D605" t="s">
+        <v>7</v>
+      </c>
+      <c r="E605" t="s">
         <v>47</v>
-      </c>
-      <c r="E605" t="s">
-        <v>48</v>
       </c>
       <c r="F605">
         <v>176</v>
@@ -17015,10 +17006,10 @@
         <v>28</v>
       </c>
       <c r="D606" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E606" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F606">
         <v>741</v>
@@ -17035,7 +17026,7 @@
         <v>10</v>
       </c>
       <c r="E607" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F607">
         <v>398</v>
@@ -17049,10 +17040,10 @@
         <v>28</v>
       </c>
       <c r="D608" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E608" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F608">
         <v>581</v>
@@ -17066,10 +17057,10 @@
         <v>29</v>
       </c>
       <c r="D609" t="s">
+        <v>7</v>
+      </c>
+      <c r="E609" t="s">
         <v>47</v>
-      </c>
-      <c r="E609" t="s">
-        <v>48</v>
       </c>
       <c r="F609">
         <v>127</v>
@@ -17083,10 +17074,10 @@
         <v>29</v>
       </c>
       <c r="D610" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E610" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F610">
         <v>630</v>
@@ -17103,7 +17094,7 @@
         <v>10</v>
       </c>
       <c r="E611" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F611">
         <v>311</v>
@@ -17117,10 +17108,10 @@
         <v>29</v>
       </c>
       <c r="D612" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E612" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F612">
         <v>389</v>
@@ -17156,7 +17147,7 @@
   <sheetData>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Se agregaron los cambios para el general
</commit_message>
<xml_diff>
--- a/Data_Cobertura_Historica.xlsx
+++ b/Data_Cobertura_Historica.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18840" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18840" windowHeight="9060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="!dData" sheetId="1" r:id="rId1"/>
-    <sheet name="!dFechas" sheetId="2" r:id="rId2"/>
+    <sheet name="!dData_Cob_Rangos" sheetId="3" r:id="rId2"/>
+    <sheet name="!dFechas" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4665" uniqueCount="57">
   <si>
     <t>Distribuidora</t>
   </si>
@@ -185,12 +186,24 @@
   <si>
     <t>COB. HIST. - GEBERAL x Mes</t>
   </si>
+  <si>
+    <t>COBERTURA RANGO TRIMESTRAL</t>
+  </si>
+  <si>
+    <t>COBERTURA RANGO SEMESTRAL</t>
+  </si>
+  <si>
+    <t>COBERTURA RANGO YTD</t>
+  </si>
+  <si>
+    <t>(KCC0) Oficina</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,8 +218,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,6 +236,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -228,18 +253,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -264,6 +294,18 @@
     <tableColumn id="3" name="Categoria"/>
     <tableColumn id="4" name="Mesa"/>
     <tableColumn id="5" name="Clientes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla10" displayName="Tabla10" ref="AF3:AH34" totalsRowShown="0">
+  <autoFilter ref="AF3:AH34"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Distribuidora"/>
+    <tableColumn id="2" name="Mesa"/>
+    <tableColumn id="3" name="Clientes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -301,6 +343,69 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Distribuidora"/>
     <tableColumn id="2" name="MES"/>
+    <tableColumn id="3" name="Clientes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="B3:E62" totalsRowShown="0">
+  <autoFilter ref="B3:E62"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Distribuidora"/>
+    <tableColumn id="2" name="Categoria"/>
+    <tableColumn id="3" name="Mesa"/>
+    <tableColumn id="4" name="Clientes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="H3:K63" totalsRowShown="0">
+  <autoFilter ref="H3:K63"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Distribuidora"/>
+    <tableColumn id="2" name="Categoria"/>
+    <tableColumn id="3" name="Mesa"/>
+    <tableColumn id="4" name="Clientes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="N3:Q67" totalsRowShown="0">
+  <autoFilter ref="N3:Q67"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Distribuidora"/>
+    <tableColumn id="2" name="Categoria"/>
+    <tableColumn id="3" name="Mesa"/>
+    <tableColumn id="4" name="Clientes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="T3:V18" totalsRowShown="0">
+  <autoFilter ref="T3:V18"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Distribuidora"/>
+    <tableColumn id="2" name="Mesa"/>
+    <tableColumn id="3" name="Clientes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="Z3:AB18" totalsRowShown="0">
+  <autoFilter ref="Z3:AB18"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Distribuidora"/>
+    <tableColumn id="2" name="Mesa"/>
     <tableColumn id="3" name="Clientes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -572,17 +677,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W612"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -600,17 +707,17 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="U1" s="1" t="s">
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="U1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -17137,10 +17244,3028 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AH67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3:AH34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="T1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="Z1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AF1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+    </row>
+    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4">
+        <v>16</v>
+      </c>
+      <c r="N4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4">
+        <v>17</v>
+      </c>
+      <c r="T4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" t="s">
+        <v>20</v>
+      </c>
+      <c r="V4">
+        <v>151</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB4">
+        <v>154</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH4">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>118</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5">
+        <v>120</v>
+      </c>
+      <c r="N5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5">
+        <v>174</v>
+      </c>
+      <c r="T5" t="s">
+        <v>5</v>
+      </c>
+      <c r="U5" t="s">
+        <v>21</v>
+      </c>
+      <c r="V5">
+        <v>2551</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB5">
+        <v>3736</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH5">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <v>71</v>
+      </c>
+      <c r="N6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6">
+        <v>95</v>
+      </c>
+      <c r="T6" t="s">
+        <v>5</v>
+      </c>
+      <c r="U6" t="s">
+        <v>22</v>
+      </c>
+      <c r="V6">
+        <v>2052</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB6">
+        <v>2694</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH6">
+        <v>2126</v>
+      </c>
+    </row>
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7">
+        <v>62</v>
+      </c>
+      <c r="N7" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7">
+        <v>74</v>
+      </c>
+      <c r="T7" t="s">
+        <v>31</v>
+      </c>
+      <c r="U7" t="s">
+        <v>33</v>
+      </c>
+      <c r="V7">
+        <v>419</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB7">
+        <v>619</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>334</v>
+      </c>
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8">
+        <v>627</v>
+      </c>
+      <c r="N8" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8">
+        <v>315</v>
+      </c>
+      <c r="T8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U8" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8">
+        <v>874</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB8">
+        <v>1042</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH8">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>2109</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9">
+        <v>3032</v>
+      </c>
+      <c r="N9" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9">
+        <v>1904</v>
+      </c>
+      <c r="T9" t="s">
+        <v>31</v>
+      </c>
+      <c r="U9" t="s">
+        <v>32</v>
+      </c>
+      <c r="V9">
+        <v>1562</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB9">
+        <v>1894</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH9">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="10" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>1468</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10">
+        <v>2542</v>
+      </c>
+      <c r="N10" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q10">
+        <v>1470</v>
+      </c>
+      <c r="T10" t="s">
+        <v>35</v>
+      </c>
+      <c r="U10" t="s">
+        <v>21</v>
+      </c>
+      <c r="V10">
+        <v>1670</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB10">
+        <v>1670</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH10">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="11" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>1343</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11">
+        <v>2064</v>
+      </c>
+      <c r="N11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q11">
+        <v>1281</v>
+      </c>
+      <c r="T11" t="s">
+        <v>36</v>
+      </c>
+      <c r="U11" t="s">
+        <v>38</v>
+      </c>
+      <c r="V11">
+        <v>2</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB11">
+        <v>5</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH11">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="12" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>303</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12">
+        <v>525</v>
+      </c>
+      <c r="N12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O12" t="s">
+        <v>7</v>
+      </c>
+      <c r="P12" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12">
+        <v>280</v>
+      </c>
+      <c r="T12" t="s">
+        <v>36</v>
+      </c>
+      <c r="U12" t="s">
+        <v>39</v>
+      </c>
+      <c r="V12">
+        <v>132</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB12">
+        <v>132</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH12">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="13" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>1746</v>
+      </c>
+      <c r="H13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13">
+        <v>2290</v>
+      </c>
+      <c r="N13" t="s">
+        <v>5</v>
+      </c>
+      <c r="O13" t="s">
+        <v>9</v>
+      </c>
+      <c r="P13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13">
+        <v>1789</v>
+      </c>
+      <c r="T13" t="s">
+        <v>36</v>
+      </c>
+      <c r="U13" t="s">
+        <v>37</v>
+      </c>
+      <c r="V13">
+        <v>1219</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB13">
+        <v>1407</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH13">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <v>1116</v>
+      </c>
+      <c r="H14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14">
+        <v>1671</v>
+      </c>
+      <c r="N14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O14" t="s">
+        <v>10</v>
+      </c>
+      <c r="P14" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q14">
+        <v>1176</v>
+      </c>
+      <c r="T14" t="s">
+        <v>41</v>
+      </c>
+      <c r="U14" t="s">
+        <v>44</v>
+      </c>
+      <c r="V14">
+        <v>1877</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB14">
+        <v>2691</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH14">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="15" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15">
+        <v>936</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15">
+        <v>1435</v>
+      </c>
+      <c r="N15" t="s">
+        <v>5</v>
+      </c>
+      <c r="O15" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15">
+        <v>948</v>
+      </c>
+      <c r="T15" t="s">
+        <v>41</v>
+      </c>
+      <c r="U15" t="s">
+        <v>45</v>
+      </c>
+      <c r="V15">
+        <v>3976</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB15">
+        <v>5330</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH15">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="16" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16">
+        <v>9</v>
+      </c>
+      <c r="N16" t="s">
+        <v>31</v>
+      </c>
+      <c r="O16" t="s">
+        <v>7</v>
+      </c>
+      <c r="P16" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q16">
+        <v>9</v>
+      </c>
+      <c r="T16" t="s">
+        <v>41</v>
+      </c>
+      <c r="U16" t="s">
+        <v>42</v>
+      </c>
+      <c r="V16">
+        <v>2869</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB16">
+        <v>4204</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH16">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="17" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17">
+        <v>388</v>
+      </c>
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17">
+        <v>588</v>
+      </c>
+      <c r="N17" t="s">
+        <v>31</v>
+      </c>
+      <c r="O17" t="s">
+        <v>9</v>
+      </c>
+      <c r="P17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q17">
+        <v>394</v>
+      </c>
+      <c r="T17" t="s">
+        <v>41</v>
+      </c>
+      <c r="U17" t="s">
+        <v>43</v>
+      </c>
+      <c r="V17">
+        <v>3243</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB17">
+        <v>4419</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH17">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="18" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18">
+        <v>14</v>
+      </c>
+      <c r="N18" t="s">
+        <v>31</v>
+      </c>
+      <c r="O18" t="s">
+        <v>10</v>
+      </c>
+      <c r="P18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q18">
+        <v>13</v>
+      </c>
+      <c r="T18" t="s">
+        <v>46</v>
+      </c>
+      <c r="U18" t="s">
+        <v>47</v>
+      </c>
+      <c r="V18">
+        <v>2297</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB18">
+        <v>2863</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19">
+        <v>205</v>
+      </c>
+      <c r="H19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19">
+        <v>307</v>
+      </c>
+      <c r="N19" t="s">
+        <v>31</v>
+      </c>
+      <c r="O19" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q19">
+        <v>217</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20">
+        <v>131</v>
+      </c>
+      <c r="H20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20">
+        <v>212</v>
+      </c>
+      <c r="N20" t="s">
+        <v>31</v>
+      </c>
+      <c r="O20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P20" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q20">
+        <v>142</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH20">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21">
+        <v>820</v>
+      </c>
+      <c r="H21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21">
+        <v>981</v>
+      </c>
+      <c r="N21" t="s">
+        <v>31</v>
+      </c>
+      <c r="O21" t="s">
+        <v>9</v>
+      </c>
+      <c r="P21" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q21">
+        <v>1015</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH21">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="22" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22">
+        <v>204</v>
+      </c>
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22">
+        <v>339</v>
+      </c>
+      <c r="N22" t="s">
+        <v>31</v>
+      </c>
+      <c r="O22" t="s">
+        <v>10</v>
+      </c>
+      <c r="P22" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q22">
+        <v>281</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23">
+        <v>556</v>
+      </c>
+      <c r="H23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23">
+        <v>697</v>
+      </c>
+      <c r="N23" t="s">
+        <v>31</v>
+      </c>
+      <c r="O23" t="s">
+        <v>11</v>
+      </c>
+      <c r="P23" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q23">
+        <v>649</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH23">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24">
+        <v>311</v>
+      </c>
+      <c r="H24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" t="s">
+        <v>32</v>
+      </c>
+      <c r="K24">
+        <v>479</v>
+      </c>
+      <c r="N24" t="s">
+        <v>31</v>
+      </c>
+      <c r="O24" t="s">
+        <v>7</v>
+      </c>
+      <c r="P24" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q24">
+        <v>329</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH24">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="25" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25">
+        <v>1400</v>
+      </c>
+      <c r="H25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25">
+        <v>1718</v>
+      </c>
+      <c r="N25" t="s">
+        <v>31</v>
+      </c>
+      <c r="O25" t="s">
+        <v>9</v>
+      </c>
+      <c r="P25" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q25">
+        <v>1731</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH25">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="26" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26">
+        <v>972</v>
+      </c>
+      <c r="H26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26">
+        <v>1322</v>
+      </c>
+      <c r="N26" t="s">
+        <v>31</v>
+      </c>
+      <c r="O26" t="s">
+        <v>10</v>
+      </c>
+      <c r="P26" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q26">
+        <v>1077</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH26">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="27" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27">
+        <v>1041</v>
+      </c>
+      <c r="H27" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27">
+        <v>1440</v>
+      </c>
+      <c r="N27" t="s">
+        <v>31</v>
+      </c>
+      <c r="O27" t="s">
+        <v>11</v>
+      </c>
+      <c r="P27" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q27">
+        <v>1235</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH27">
+        <v>2730</v>
+      </c>
+    </row>
+    <row r="28" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28">
+        <v>141</v>
+      </c>
+      <c r="H28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28">
+        <v>141</v>
+      </c>
+      <c r="N28" t="s">
+        <v>35</v>
+      </c>
+      <c r="O28" t="s">
+        <v>7</v>
+      </c>
+      <c r="P28" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q28">
+        <v>187</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH28">
+        <v>3408</v>
+      </c>
+    </row>
+    <row r="29" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29">
+        <v>1553</v>
+      </c>
+      <c r="H29" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29">
+        <v>1553</v>
+      </c>
+      <c r="N29" t="s">
+        <v>35</v>
+      </c>
+      <c r="O29" t="s">
+        <v>9</v>
+      </c>
+      <c r="P29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q29">
+        <v>1825</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH29">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="30" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30">
+        <v>421</v>
+      </c>
+      <c r="H30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30">
+        <v>421</v>
+      </c>
+      <c r="N30" t="s">
+        <v>35</v>
+      </c>
+      <c r="O30" t="s">
+        <v>10</v>
+      </c>
+      <c r="P30" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q30">
+        <v>555</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH30">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="31" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31">
+        <v>950</v>
+      </c>
+      <c r="H31" t="s">
+        <v>35</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31">
+        <v>950</v>
+      </c>
+      <c r="N31" t="s">
+        <v>35</v>
+      </c>
+      <c r="O31" t="s">
+        <v>11</v>
+      </c>
+      <c r="P31" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q31">
+        <v>1095</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH31">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="32" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>36</v>
+      </c>
+      <c r="I32" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" t="s">
+        <v>38</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+      <c r="N32" t="s">
+        <v>36</v>
+      </c>
+      <c r="O32" t="s">
+        <v>7</v>
+      </c>
+      <c r="P32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH32">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="33" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="H33" t="s">
+        <v>36</v>
+      </c>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" t="s">
+        <v>38</v>
+      </c>
+      <c r="K33">
+        <v>3</v>
+      </c>
+      <c r="N33" t="s">
+        <v>36</v>
+      </c>
+      <c r="O33" t="s">
+        <v>9</v>
+      </c>
+      <c r="P33" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH33">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="34" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>36</v>
+      </c>
+      <c r="I34" t="s">
+        <v>10</v>
+      </c>
+      <c r="J34" t="s">
+        <v>38</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="N34" t="s">
+        <v>36</v>
+      </c>
+      <c r="O34" t="s">
+        <v>10</v>
+      </c>
+      <c r="P34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH34">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="35" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35">
+        <v>48</v>
+      </c>
+      <c r="H35" t="s">
+        <v>36</v>
+      </c>
+      <c r="I35" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K35">
+        <v>5</v>
+      </c>
+      <c r="N35" t="s">
+        <v>36</v>
+      </c>
+      <c r="O35" t="s">
+        <v>11</v>
+      </c>
+      <c r="P35" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36">
+        <v>92</v>
+      </c>
+      <c r="H36" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" t="s">
+        <v>39</v>
+      </c>
+      <c r="K36">
+        <v>48</v>
+      </c>
+      <c r="N36" t="s">
+        <v>36</v>
+      </c>
+      <c r="O36" t="s">
+        <v>7</v>
+      </c>
+      <c r="P36" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37">
+        <v>50</v>
+      </c>
+      <c r="H37" t="s">
+        <v>36</v>
+      </c>
+      <c r="I37" t="s">
+        <v>9</v>
+      </c>
+      <c r="J37" t="s">
+        <v>39</v>
+      </c>
+      <c r="K37">
+        <v>92</v>
+      </c>
+      <c r="N37" t="s">
+        <v>36</v>
+      </c>
+      <c r="O37" t="s">
+        <v>9</v>
+      </c>
+      <c r="P37" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38">
+        <v>82</v>
+      </c>
+      <c r="H38" t="s">
+        <v>36</v>
+      </c>
+      <c r="I38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J38" t="s">
+        <v>39</v>
+      </c>
+      <c r="K38">
+        <v>50</v>
+      </c>
+      <c r="N38" t="s">
+        <v>36</v>
+      </c>
+      <c r="O38" t="s">
+        <v>10</v>
+      </c>
+      <c r="P38" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39">
+        <v>224</v>
+      </c>
+      <c r="H39" t="s">
+        <v>36</v>
+      </c>
+      <c r="I39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" t="s">
+        <v>39</v>
+      </c>
+      <c r="K39">
+        <v>82</v>
+      </c>
+      <c r="N39" t="s">
+        <v>36</v>
+      </c>
+      <c r="O39" t="s">
+        <v>11</v>
+      </c>
+      <c r="P39" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40">
+        <v>1117</v>
+      </c>
+      <c r="H40" t="s">
+        <v>36</v>
+      </c>
+      <c r="I40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" t="s">
+        <v>37</v>
+      </c>
+      <c r="K40">
+        <v>275</v>
+      </c>
+      <c r="N40" t="s">
+        <v>36</v>
+      </c>
+      <c r="O40" t="s">
+        <v>7</v>
+      </c>
+      <c r="P40" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q40">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41">
+        <v>432</v>
+      </c>
+      <c r="H41" t="s">
+        <v>36</v>
+      </c>
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
+      <c r="J41" t="s">
+        <v>37</v>
+      </c>
+      <c r="K41">
+        <v>1300</v>
+      </c>
+      <c r="N41" t="s">
+        <v>36</v>
+      </c>
+      <c r="O41" t="s">
+        <v>9</v>
+      </c>
+      <c r="P41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q41">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42">
+        <v>674</v>
+      </c>
+      <c r="H42" t="s">
+        <v>36</v>
+      </c>
+      <c r="I42" t="s">
+        <v>10</v>
+      </c>
+      <c r="J42" t="s">
+        <v>37</v>
+      </c>
+      <c r="K42">
+        <v>507</v>
+      </c>
+      <c r="N42" t="s">
+        <v>36</v>
+      </c>
+      <c r="O42" t="s">
+        <v>10</v>
+      </c>
+      <c r="P42" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q42">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43">
+        <v>60</v>
+      </c>
+      <c r="H43" t="s">
+        <v>36</v>
+      </c>
+      <c r="I43" t="s">
+        <v>11</v>
+      </c>
+      <c r="J43" t="s">
+        <v>37</v>
+      </c>
+      <c r="K43">
+        <v>789</v>
+      </c>
+      <c r="N43" t="s">
+        <v>36</v>
+      </c>
+      <c r="O43" t="s">
+        <v>11</v>
+      </c>
+      <c r="P43" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q43">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44">
+        <v>1657</v>
+      </c>
+      <c r="H44" t="s">
+        <v>41</v>
+      </c>
+      <c r="I44" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" t="s">
+        <v>44</v>
+      </c>
+      <c r="K44">
+        <v>138</v>
+      </c>
+      <c r="N44" t="s">
+        <v>36</v>
+      </c>
+      <c r="O44" t="s">
+        <v>7</v>
+      </c>
+      <c r="P44" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q44">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="45" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45">
+        <v>667</v>
+      </c>
+      <c r="H45" t="s">
+        <v>41</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
+      <c r="J45" t="s">
+        <v>44</v>
+      </c>
+      <c r="K45">
+        <v>2383</v>
+      </c>
+      <c r="N45" t="s">
+        <v>36</v>
+      </c>
+      <c r="O45" t="s">
+        <v>9</v>
+      </c>
+      <c r="P45" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q45">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="46" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46">
+        <v>532</v>
+      </c>
+      <c r="H46" t="s">
+        <v>41</v>
+      </c>
+      <c r="I46" t="s">
+        <v>10</v>
+      </c>
+      <c r="J46" t="s">
+        <v>44</v>
+      </c>
+      <c r="K46">
+        <v>1198</v>
+      </c>
+      <c r="N46" t="s">
+        <v>36</v>
+      </c>
+      <c r="O46" t="s">
+        <v>10</v>
+      </c>
+      <c r="P46" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q46">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="47" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>45</v>
+      </c>
+      <c r="E47">
+        <v>117</v>
+      </c>
+      <c r="H47" t="s">
+        <v>41</v>
+      </c>
+      <c r="I47" t="s">
+        <v>11</v>
+      </c>
+      <c r="J47" t="s">
+        <v>44</v>
+      </c>
+      <c r="K47">
+        <v>860</v>
+      </c>
+      <c r="N47" t="s">
+        <v>36</v>
+      </c>
+      <c r="O47" t="s">
+        <v>11</v>
+      </c>
+      <c r="P47" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q47">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="48" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48">
+        <v>3521</v>
+      </c>
+      <c r="H48" t="s">
+        <v>41</v>
+      </c>
+      <c r="I48" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" t="s">
+        <v>45</v>
+      </c>
+      <c r="K48">
+        <v>189</v>
+      </c>
+      <c r="N48" t="s">
+        <v>41</v>
+      </c>
+      <c r="O48" t="s">
+        <v>7</v>
+      </c>
+      <c r="P48" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q48">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>45</v>
+      </c>
+      <c r="E49">
+        <v>1463</v>
+      </c>
+      <c r="H49" t="s">
+        <v>41</v>
+      </c>
+      <c r="I49" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49" t="s">
+        <v>45</v>
+      </c>
+      <c r="K49">
+        <v>4748</v>
+      </c>
+      <c r="N49" t="s">
+        <v>41</v>
+      </c>
+      <c r="O49" t="s">
+        <v>9</v>
+      </c>
+      <c r="P49" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q49">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50">
+        <v>1037</v>
+      </c>
+      <c r="H50" t="s">
+        <v>41</v>
+      </c>
+      <c r="I50" t="s">
+        <v>10</v>
+      </c>
+      <c r="J50" t="s">
+        <v>45</v>
+      </c>
+      <c r="K50">
+        <v>2180</v>
+      </c>
+      <c r="N50" t="s">
+        <v>41</v>
+      </c>
+      <c r="O50" t="s">
+        <v>10</v>
+      </c>
+      <c r="P50" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q50">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51">
+        <v>339</v>
+      </c>
+      <c r="H51" t="s">
+        <v>41</v>
+      </c>
+      <c r="I51" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" t="s">
+        <v>45</v>
+      </c>
+      <c r="K51">
+        <v>1539</v>
+      </c>
+      <c r="N51" t="s">
+        <v>41</v>
+      </c>
+      <c r="O51" t="s">
+        <v>11</v>
+      </c>
+      <c r="P51" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q51">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52">
+        <v>2545</v>
+      </c>
+      <c r="H52" t="s">
+        <v>41</v>
+      </c>
+      <c r="I52" t="s">
+        <v>7</v>
+      </c>
+      <c r="J52" t="s">
+        <v>42</v>
+      </c>
+      <c r="K52">
+        <v>597</v>
+      </c>
+      <c r="N52" t="s">
+        <v>41</v>
+      </c>
+      <c r="O52" t="s">
+        <v>7</v>
+      </c>
+      <c r="P52" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q52">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53">
+        <v>957</v>
+      </c>
+      <c r="H53" t="s">
+        <v>41</v>
+      </c>
+      <c r="I53" t="s">
+        <v>9</v>
+      </c>
+      <c r="J53" t="s">
+        <v>42</v>
+      </c>
+      <c r="K53">
+        <v>3666</v>
+      </c>
+      <c r="N53" t="s">
+        <v>41</v>
+      </c>
+      <c r="O53" t="s">
+        <v>9</v>
+      </c>
+      <c r="P53" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q53">
+        <v>3959</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54">
+        <v>1346</v>
+      </c>
+      <c r="H54" t="s">
+        <v>41</v>
+      </c>
+      <c r="I54" t="s">
+        <v>10</v>
+      </c>
+      <c r="J54" t="s">
+        <v>42</v>
+      </c>
+      <c r="K54">
+        <v>1761</v>
+      </c>
+      <c r="N54" t="s">
+        <v>41</v>
+      </c>
+      <c r="O54" t="s">
+        <v>10</v>
+      </c>
+      <c r="P54" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q54">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>43</v>
+      </c>
+      <c r="E55">
+        <v>150</v>
+      </c>
+      <c r="H55" t="s">
+        <v>41</v>
+      </c>
+      <c r="I55" t="s">
+        <v>11</v>
+      </c>
+      <c r="J55" t="s">
+        <v>42</v>
+      </c>
+      <c r="K55">
+        <v>2494</v>
+      </c>
+      <c r="N55" t="s">
+        <v>41</v>
+      </c>
+      <c r="O55" t="s">
+        <v>11</v>
+      </c>
+      <c r="P55" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q55">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>43</v>
+      </c>
+      <c r="E56">
+        <v>2790</v>
+      </c>
+      <c r="H56" t="s">
+        <v>41</v>
+      </c>
+      <c r="I56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J56" t="s">
+        <v>43</v>
+      </c>
+      <c r="K56">
+        <v>285</v>
+      </c>
+      <c r="N56" t="s">
+        <v>41</v>
+      </c>
+      <c r="O56" t="s">
+        <v>7</v>
+      </c>
+      <c r="P56" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q56">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57">
+        <v>1038</v>
+      </c>
+      <c r="H57" t="s">
+        <v>41</v>
+      </c>
+      <c r="I57" t="s">
+        <v>9</v>
+      </c>
+      <c r="J57" t="s">
+        <v>43</v>
+      </c>
+      <c r="K57">
+        <v>3794</v>
+      </c>
+      <c r="N57" t="s">
+        <v>41</v>
+      </c>
+      <c r="O57" t="s">
+        <v>9</v>
+      </c>
+      <c r="P57" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q57">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58">
+        <v>910</v>
+      </c>
+      <c r="H58" t="s">
+        <v>41</v>
+      </c>
+      <c r="I58" t="s">
+        <v>10</v>
+      </c>
+      <c r="J58" t="s">
+        <v>43</v>
+      </c>
+      <c r="K58">
+        <v>1553</v>
+      </c>
+      <c r="N58" t="s">
+        <v>41</v>
+      </c>
+      <c r="O58" t="s">
+        <v>10</v>
+      </c>
+      <c r="P58" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q58">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>47</v>
+      </c>
+      <c r="E59">
+        <v>489</v>
+      </c>
+      <c r="H59" t="s">
+        <v>41</v>
+      </c>
+      <c r="I59" t="s">
+        <v>11</v>
+      </c>
+      <c r="J59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K59">
+        <v>1418</v>
+      </c>
+      <c r="N59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O59" t="s">
+        <v>11</v>
+      </c>
+      <c r="P59" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q59">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" t="s">
+        <v>47</v>
+      </c>
+      <c r="E60">
+        <v>1867</v>
+      </c>
+      <c r="H60" t="s">
+        <v>46</v>
+      </c>
+      <c r="I60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J60" t="s">
+        <v>47</v>
+      </c>
+      <c r="K60">
+        <v>850</v>
+      </c>
+      <c r="N60" t="s">
+        <v>41</v>
+      </c>
+      <c r="O60" t="s">
+        <v>7</v>
+      </c>
+      <c r="P60" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q60">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" t="s">
+        <v>47</v>
+      </c>
+      <c r="E61">
+        <v>995</v>
+      </c>
+      <c r="H61" t="s">
+        <v>46</v>
+      </c>
+      <c r="I61" t="s">
+        <v>9</v>
+      </c>
+      <c r="J61" t="s">
+        <v>47</v>
+      </c>
+      <c r="K61">
+        <v>2447</v>
+      </c>
+      <c r="N61" t="s">
+        <v>41</v>
+      </c>
+      <c r="O61" t="s">
+        <v>9</v>
+      </c>
+      <c r="P61" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q61">
+        <v>2924</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>46</v>
+      </c>
+      <c r="C62" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" t="s">
+        <v>47</v>
+      </c>
+      <c r="E62">
+        <v>1266</v>
+      </c>
+      <c r="H62" t="s">
+        <v>46</v>
+      </c>
+      <c r="I62" t="s">
+        <v>10</v>
+      </c>
+      <c r="J62" t="s">
+        <v>47</v>
+      </c>
+      <c r="K62">
+        <v>1698</v>
+      </c>
+      <c r="N62" t="s">
+        <v>41</v>
+      </c>
+      <c r="O62" t="s">
+        <v>10</v>
+      </c>
+      <c r="P62" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q62">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>46</v>
+      </c>
+      <c r="I63" t="s">
+        <v>11</v>
+      </c>
+      <c r="J63" t="s">
+        <v>47</v>
+      </c>
+      <c r="K63">
+        <v>1862</v>
+      </c>
+      <c r="N63" t="s">
+        <v>41</v>
+      </c>
+      <c r="O63" t="s">
+        <v>11</v>
+      </c>
+      <c r="P63" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q63">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N64" t="s">
+        <v>46</v>
+      </c>
+      <c r="O64" t="s">
+        <v>7</v>
+      </c>
+      <c r="P64" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q64">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="65" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N65" t="s">
+        <v>46</v>
+      </c>
+      <c r="O65" t="s">
+        <v>9</v>
+      </c>
+      <c r="P65" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q65">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="66" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N66" t="s">
+        <v>46</v>
+      </c>
+      <c r="O66" t="s">
+        <v>10</v>
+      </c>
+      <c r="P66" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q66">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="67" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N67" t="s">
+        <v>46</v>
+      </c>
+      <c r="O67" t="s">
+        <v>11</v>
+      </c>
+      <c r="P67" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q67">
+        <v>1213</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AF1:AH1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="6">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se corrgieron los datos para el crecimiento general
</commit_message>
<xml_diff>
--- a/Data_Cobertura_Historica.xlsx
+++ b/Data_Cobertura_Historica.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4665" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4635" uniqueCount="56">
   <si>
     <t>Distribuidora</t>
   </si>
@@ -195,9 +195,6 @@
   <si>
     <t>COBERTURA RANGO YTD</t>
   </si>
-  <si>
-    <t>(KCC0) Oficina</t>
-  </si>
 </sst>
 </file>
 
@@ -300,8 +297,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla10" displayName="Tabla10" ref="AF3:AH34" totalsRowShown="0">
-  <autoFilter ref="AF3:AH34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla10" displayName="Tabla10" ref="AF3:AH19" totalsRowShown="0">
+  <autoFilter ref="AF3:AH19"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Distribuidora"/>
     <tableColumn id="2" name="Mesa"/>
@@ -17246,9 +17243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AH67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3:AH34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17427,7 +17422,7 @@
         <v>20</v>
       </c>
       <c r="AH4">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="2:34" x14ac:dyDescent="0.25">
@@ -17492,7 +17487,7 @@
         <v>21</v>
       </c>
       <c r="AH5">
-        <v>2375</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="6" spans="2:34" x14ac:dyDescent="0.25">
@@ -17557,7 +17552,7 @@
         <v>22</v>
       </c>
       <c r="AH6">
-        <v>2126</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="7" spans="2:34" x14ac:dyDescent="0.25">
@@ -17616,13 +17611,13 @@
         <v>619</v>
       </c>
       <c r="AF7" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="AG7" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="AH7">
-        <v>2</v>
+        <v>471</v>
       </c>
     </row>
     <row r="8" spans="2:34" x14ac:dyDescent="0.25">
@@ -17681,13 +17676,13 @@
         <v>1042</v>
       </c>
       <c r="AF8" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="AG8" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="AH8">
-        <v>1707</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="9" spans="2:34" x14ac:dyDescent="0.25">
@@ -17746,13 +17741,13 @@
         <v>1894</v>
       </c>
       <c r="AF9" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="AG9" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AH9">
-        <v>1059</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="10" spans="2:34" x14ac:dyDescent="0.25">
@@ -17811,13 +17806,13 @@
         <v>1670</v>
       </c>
       <c r="AF10" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AG10" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="AH10">
-        <v>422</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="11" spans="2:34" x14ac:dyDescent="0.25">
@@ -17876,13 +17871,13 @@
         <v>5</v>
       </c>
       <c r="AF11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="AG11" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="AH11">
-        <v>1102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:34" x14ac:dyDescent="0.25">
@@ -17941,13 +17936,13 @@
         <v>132</v>
       </c>
       <c r="AF12" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="AG12" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="AH12">
-        <v>1935</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:34" x14ac:dyDescent="0.25">
@@ -18006,13 +18001,13 @@
         <v>1407</v>
       </c>
       <c r="AF13" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="AG13" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="AH13">
-        <v>201</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="2:34" x14ac:dyDescent="0.25">
@@ -18071,13 +18066,13 @@
         <v>2691</v>
       </c>
       <c r="AF14" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="AG14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="AH14">
-        <v>370</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="15" spans="2:34" x14ac:dyDescent="0.25">
@@ -18136,13 +18131,13 @@
         <v>5330</v>
       </c>
       <c r="AF15" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="AG15" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="AH15">
-        <v>1290</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="16" spans="2:34" x14ac:dyDescent="0.25">
@@ -18201,13 +18196,13 @@
         <v>4204</v>
       </c>
       <c r="AF16" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="AG16" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="AH16">
-        <v>1960</v>
+        <v>5088</v>
       </c>
     </row>
     <row r="17" spans="2:34" x14ac:dyDescent="0.25">
@@ -18266,13 +18261,13 @@
         <v>4419</v>
       </c>
       <c r="AF17" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="AG17" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="AH17">
-        <v>1345</v>
+        <v>3112</v>
       </c>
     </row>
     <row r="18" spans="2:34" x14ac:dyDescent="0.25">
@@ -18331,13 +18326,13 @@
         <v>2863</v>
       </c>
       <c r="AF18" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="AG18" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="AH18">
-        <v>1</v>
+        <v>3734</v>
       </c>
     </row>
     <row r="19" spans="2:34" x14ac:dyDescent="0.25">
@@ -18378,13 +18373,13 @@
         <v>217</v>
       </c>
       <c r="AF19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="AG19" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="AH19">
-        <v>6</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="20" spans="2:34" x14ac:dyDescent="0.25">
@@ -18424,15 +18419,6 @@
       <c r="Q20">
         <v>142</v>
       </c>
-      <c r="AF20" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH20">
-        <v>142</v>
-      </c>
     </row>
     <row r="21" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -18471,15 +18457,6 @@
       <c r="Q21">
         <v>1015</v>
       </c>
-      <c r="AF21" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG21" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH21">
-        <v>1191</v>
-      </c>
     </row>
     <row r="22" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
@@ -18518,15 +18495,6 @@
       <c r="Q22">
         <v>281</v>
       </c>
-      <c r="AF22" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG22" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH22">
-        <v>1</v>
-      </c>
     </row>
     <row r="23" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -18565,15 +18533,6 @@
       <c r="Q23">
         <v>649</v>
       </c>
-      <c r="AF23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG23" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH23">
-        <v>106</v>
-      </c>
     </row>
     <row r="24" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -18612,15 +18571,6 @@
       <c r="Q24">
         <v>329</v>
       </c>
-      <c r="AF24" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG24" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH24">
-        <v>647</v>
-      </c>
     </row>
     <row r="25" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
@@ -18659,15 +18609,6 @@
       <c r="Q25">
         <v>1731</v>
       </c>
-      <c r="AF25" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG25" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH25">
-        <v>2058</v>
-      </c>
     </row>
     <row r="26" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -18706,15 +18647,6 @@
       <c r="Q26">
         <v>1077</v>
       </c>
-      <c r="AF26" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG26" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH26">
-        <v>4581</v>
-      </c>
     </row>
     <row r="27" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -18752,15 +18684,6 @@
       </c>
       <c r="Q27">
         <v>1235</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG27" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH27">
-        <v>2730</v>
       </c>
     </row>
     <row r="28" spans="2:34" x14ac:dyDescent="0.25">
@@ -18800,15 +18723,6 @@
       <c r="Q28">
         <v>187</v>
       </c>
-      <c r="AF28" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG28" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH28">
-        <v>3408</v>
-      </c>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -18847,15 +18761,6 @@
       <c r="Q29">
         <v>1825</v>
       </c>
-      <c r="AF29" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG29" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH29">
-        <v>835</v>
-      </c>
     </row>
     <row r="30" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -18894,15 +18799,6 @@
       <c r="Q30">
         <v>555</v>
       </c>
-      <c r="AF30" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG30" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH30">
-        <v>1976</v>
-      </c>
     </row>
     <row r="31" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -18941,15 +18837,6 @@
       <c r="Q31">
         <v>1095</v>
       </c>
-      <c r="AF31" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG31" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH31">
-        <v>1395</v>
-      </c>
     </row>
     <row r="32" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
@@ -18988,17 +18875,8 @@
       <c r="Q32">
         <v>1</v>
       </c>
-      <c r="AF32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG32" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH32">
-        <v>1188</v>
-      </c>
-    </row>
-    <row r="33" spans="2:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>36</v>
       </c>
@@ -19035,17 +18913,8 @@
       <c r="Q33">
         <v>1</v>
       </c>
-      <c r="AF33" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG33" t="s">
-        <v>47</v>
-      </c>
-      <c r="AH33">
-        <v>2233</v>
-      </c>
-    </row>
-    <row r="34" spans="2:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>36</v>
       </c>
@@ -19082,17 +18951,8 @@
       <c r="Q34">
         <v>1</v>
       </c>
-      <c r="AF34" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG34" t="s">
-        <v>47</v>
-      </c>
-      <c r="AH34">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="35" spans="2:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>36</v>
       </c>
@@ -19130,7 +18990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>36</v>
       </c>
@@ -19168,7 +19028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -19206,7 +19066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>36</v>
       </c>
@@ -19244,7 +19104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>36</v>
       </c>
@@ -19282,7 +19142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>36</v>
       </c>
@@ -19320,7 +19180,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>36</v>
       </c>
@@ -19358,7 +19218,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>36</v>
       </c>
@@ -19396,7 +19256,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>41</v>
       </c>
@@ -19434,7 +19294,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>41</v>
       </c>
@@ -19472,7 +19332,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="45" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>41</v>
       </c>
@@ -19510,7 +19370,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="46" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>41</v>
       </c>
@@ -19548,7 +19408,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="47" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>41</v>
       </c>
@@ -19586,7 +19446,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="48" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>41</v>
       </c>
@@ -20240,12 +20100,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Eliminado el KCC0 de ANGELIKA
</commit_message>
<xml_diff>
--- a/Data_Cobertura_Historica.xlsx
+++ b/Data_Cobertura_Historica.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4635" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4635" uniqueCount="55">
   <si>
     <t>Distribuidora</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>COBERTURA RANGO YTD</t>
-  </si>
-  <si>
-    <t>(KCC0) Oficina</t>
   </si>
 </sst>
 </file>
@@ -674,7 +671,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W612"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6074,7 +6073,7 @@
         <v>9</v>
       </c>
       <c r="E117" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -6279,7 +6278,7 @@
         <v>11</v>
       </c>
       <c r="E122" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F122">
         <v>1</v>

</xml_diff>